<commit_message>
Mod updates & Minetweaker scripts
</commit_message>
<xml_diff>
--- a/Modlist.xlsx
+++ b/Modlist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="506">
   <si>
     <t>Mod</t>
   </si>
@@ -318,9 +318,6 @@
     <t>MobiusCore</t>
   </si>
   <si>
-    <t>Opis</t>
-  </si>
-  <si>
     <t>Mineshopper</t>
   </si>
   <si>
@@ -930,9 +927,6 @@
     <t>4.0.1</t>
   </si>
   <si>
-    <t>rv1-stable-1</t>
-  </si>
-  <si>
     <t>Realistic World Generation</t>
   </si>
   <si>
@@ -1035,12 +1029,6 @@
     <t>Ivorforce</t>
   </si>
   <si>
-    <t>0.11.0.4-QMX</t>
-  </si>
-  <si>
-    <t>0.4.0.100</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -1365,9 +1353,6 @@
     <t>1.3.0b-3</t>
   </si>
   <si>
-    <t>2.3.3-28</t>
-  </si>
-  <si>
     <t>1.15</t>
   </si>
   <si>
@@ -1452,12 +1437,6 @@
     <t>1.2.2-b66</t>
   </si>
   <si>
-    <t>2.9</t>
-  </si>
-  <si>
-    <t>1.2.4c-6</t>
-  </si>
-  <si>
     <t>a-1.3.0.1</t>
   </si>
   <si>
@@ -1474,6 +1453,87 @@
   </si>
   <si>
     <t>1.3.3-25</t>
+  </si>
+  <si>
+    <t>Ztones</t>
+  </si>
+  <si>
+    <t>http://www.minecraftforum.net/forums/mapping-and-modding/minecraft-mods/2221070-ztones-v-2-2-1-decorative-blocks-16x</t>
+  </si>
+  <si>
+    <t>RiciJak</t>
+  </si>
+  <si>
+    <t>2.2.1</t>
+  </si>
+  <si>
+    <t>http://minecraft.curseforge.com/mc-mods/224663-openmodularturrets</t>
+  </si>
+  <si>
+    <t>Pounjabisous</t>
+  </si>
+  <si>
+    <t>1.2.4c</t>
+  </si>
+  <si>
+    <t>rv2-beta-8</t>
+  </si>
+  <si>
+    <t>Antique Atlas</t>
+  </si>
+  <si>
+    <t>Hunternif</t>
+  </si>
+  <si>
+    <t>http://www.minecraftforum.net/forums/mapping-and-modding/minecraft-mods/1292324-1-7-2-1-6-4-1-5-2-forge-antique-atlas</t>
+  </si>
+  <si>
+    <t>4.0.1a</t>
+  </si>
+  <si>
+    <t>2.3.5.31</t>
+  </si>
+  <si>
+    <t>2.10</t>
+  </si>
+  <si>
+    <t>0.4.0.5-QMX</t>
+  </si>
+  <si>
+    <t>0.11.0.5-QMX</t>
+  </si>
+  <si>
+    <t>AnimationAPI</t>
+  </si>
+  <si>
+    <t>1.2.4</t>
+  </si>
+  <si>
+    <t>OggAudioData</t>
+  </si>
+  <si>
+    <t>Player API Core</t>
+  </si>
+  <si>
+    <t>Smart Moving</t>
+  </si>
+  <si>
+    <t>http://www.minecraftforum.net/forums/mapping-and-modding/minecraft-mods/1274224-smart-moving</t>
+  </si>
+  <si>
+    <t>15.2</t>
+  </si>
+  <si>
+    <t>Divisor</t>
+  </si>
+  <si>
+    <t>RC6-B</t>
+  </si>
+  <si>
+    <t>http://www.minecraftforum.net/forums/mapping-and-modding/minecraft-mods/1277996-1-8-api-player-api</t>
+  </si>
+  <si>
+    <t>http://www.minecraftforum.net/forums/mapping-and-modding/minecraft-mods/1283669-1-8-api-render-player-api</t>
   </si>
 </sst>
 </file>
@@ -1985,11 +2045,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F152"/>
+  <dimension ref="A1:F157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C108" sqref="C108"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2018,7 +2078,7 @@
         <v>30</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2026,7 +2086,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
@@ -2041,7 +2101,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -2056,7 +2116,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>7</v>
@@ -2068,25 +2128,25 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E5" s="23"/>
     </row>
     <row r="6" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>26</v>
@@ -2101,7 +2161,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>27</v>
@@ -2113,10 +2173,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>27</v>
@@ -2130,7 +2190,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>84</v>
@@ -2145,7 +2205,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -2157,16 +2217,16 @@
     </row>
     <row r="11" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="28" t="s">
         <v>143</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>280</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>144</v>
       </c>
       <c r="E11" s="18"/>
     </row>
@@ -2175,43 +2235,43 @@
         <v>99</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>39</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E14" s="18"/>
     </row>
@@ -2220,7 +2280,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>340</v>
+        <v>493</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>50</v>
@@ -2232,10 +2292,10 @@
     </row>
     <row r="16" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>50</v>
@@ -2247,1996 +2307,1993 @@
     </row>
     <row r="17" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>343</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>344</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>471</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>474</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>473</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>472</v>
+        <v>497</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="28"/>
+    </row>
+    <row r="18" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>495</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>306</v>
+        <v>498</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>477</v>
+        <v>459</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>277</v>
+        <v>502</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>307</v>
-      </c>
-      <c r="E19" s="18"/>
+        <v>504</v>
+      </c>
     </row>
     <row r="20" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>420</v>
+        <v>339</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>421</v>
+        <v>340</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>423</v>
+        <v>336</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>422</v>
-      </c>
-      <c r="E20" s="18"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>466</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>469</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>472</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>305</v>
+      </c>
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>416</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>417</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>418</v>
+      </c>
+      <c r="E23" s="18"/>
+    </row>
+    <row r="24" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="18" t="s">
+        <v>487</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>490</v>
+      </c>
+      <c r="C24" t="s">
+        <v>488</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>489</v>
+      </c>
+      <c r="E24" s="18"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B21" s="18" t="s">
-        <v>355</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="D25" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="D21" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="E21" s="22"/>
-    </row>
-    <row r="22" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="E25" s="22"/>
+    </row>
+    <row r="26" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="18" t="s">
-        <v>393</v>
-      </c>
-      <c r="C22" s="4" t="s">
+      <c r="B26" s="18" t="s">
+        <v>389</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D26" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="E22" s="21"/>
-    </row>
-    <row r="23" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>411</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>413</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>412</v>
-      </c>
-      <c r="E23" s="21"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>304</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="E24" s="22"/>
-    </row>
-    <row r="25" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>285</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="D25" s="28" t="s">
-        <v>188</v>
-      </c>
-      <c r="E25" s="18"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>322</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" s="22"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>15</v>
+      <c r="E26" s="21"/>
+    </row>
+    <row r="27" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>406</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>295</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D27" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="E27" s="22"/>
+        <v>407</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>408</v>
+      </c>
+      <c r="E27" s="21"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>16</v>
+        <v>224</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>323</v>
+        <v>486</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" s="22"/>
+    </row>
+    <row r="29" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="E29" s="18"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D30" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="E28" s="22"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>324</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D29" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="E29" s="22"/>
-    </row>
-    <row r="30" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D30" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E30" s="18"/>
+      <c r="E30" s="22"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>366</v>
+        <v>294</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E31" s="22"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>448</v>
+        <v>321</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E32" s="22"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>482</v>
+        <v>322</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>294</v>
+        <v>92</v>
       </c>
       <c r="D33" s="27" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E33" s="22"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>440</v>
+    <row r="34" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>195</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>447</v>
+        <v>359</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>441</v>
-      </c>
-      <c r="D34" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="E34" s="22"/>
-    </row>
-    <row r="35" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>21</v>
+        <v>197</v>
+      </c>
+      <c r="D34" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="E34" s="18"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>445</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>438</v>
-      </c>
-      <c r="D35" s="28" t="s">
-        <v>437</v>
-      </c>
-      <c r="E35" s="18"/>
+        <v>362</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35" s="22"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>348</v>
+        <v>444</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E36" s="22"/>
     </row>
-    <row r="37" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>23</v>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="E37" s="18"/>
+        <v>475</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="D37" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="E37" s="22"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>317</v>
+        <v>436</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>449</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>316</v>
+        <v>443</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>437</v>
       </c>
       <c r="D38" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="E38" s="22"/>
+    </row>
+    <row r="39" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>441</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="D39" s="28" t="s">
+        <v>433</v>
+      </c>
+      <c r="E39" s="18"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D40" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="E40" s="22"/>
+    </row>
+    <row r="41" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="E41" s="18"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="E38" s="22"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="B39" s="18" t="s">
-        <v>478</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="D39" s="27" t="s">
-        <v>361</v>
-      </c>
-      <c r="E39" s="22"/>
-    </row>
-    <row r="40" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>367</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>365</v>
-      </c>
-      <c r="D40" s="28" t="s">
-        <v>364</v>
-      </c>
-      <c r="E40" s="18"/>
-    </row>
-    <row r="41" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="D41" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="E41" s="20"/>
-    </row>
-    <row r="42" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="B42" s="21" t="s">
-        <v>450</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>331</v>
-      </c>
-      <c r="D42" s="31" t="s">
-        <v>330</v>
-      </c>
-      <c r="E42" s="21"/>
-    </row>
-    <row r="43" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>28</v>
+      <c r="B42" s="18" t="s">
+        <v>491</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="D42" s="27" t="s">
+        <v>313</v>
+      </c>
+      <c r="E42" s="22"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>358</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>373</v>
+        <v>492</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D43" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="E43" s="18"/>
+        <v>398</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>357</v>
+      </c>
+      <c r="E43" s="22"/>
     </row>
     <row r="44" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="D44" s="28" t="s">
+        <v>360</v>
+      </c>
+      <c r="E44" s="18"/>
+    </row>
+    <row r="45" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B45" s="20"/>
+      <c r="C45" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D45" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="E45" s="20"/>
+    </row>
+    <row r="46" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>445</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="D46" s="31" t="s">
+        <v>328</v>
+      </c>
+      <c r="E46" s="21"/>
+    </row>
+    <row r="47" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" s="18" t="s">
+        <v>369</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D47" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="E47" s="18"/>
+    </row>
+    <row r="48" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="B44" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="C44" s="4" t="s">
+      <c r="D48" s="27" t="s">
         <v>277</v>
       </c>
-      <c r="D44" s="27" t="s">
-        <v>278</v>
-      </c>
-      <c r="E44" s="18"/>
-    </row>
-    <row r="45" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>461</v>
-      </c>
-      <c r="B45" s="18" t="s">
-        <v>464</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>463</v>
-      </c>
-      <c r="D45" s="27" t="s">
-        <v>462</v>
-      </c>
-      <c r="E45" s="18"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B46" s="18" t="s">
-        <v>235</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D46" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="E46" s="22"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="B47" s="18" t="s">
-        <v>264</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D47" s="27" t="s">
-        <v>259</v>
-      </c>
-      <c r="E47" s="22"/>
-    </row>
-    <row r="48" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="B48" s="20"/>
-      <c r="C48" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="D48" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="E48" s="20"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>167</v>
+      <c r="E48" s="18"/>
+    </row>
+    <row r="49" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>456</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>171</v>
+        <v>459</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>458</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>170</v>
-      </c>
-      <c r="E49" s="22"/>
+        <v>457</v>
+      </c>
+      <c r="E49" s="18"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>374</v>
+        <v>31</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>434</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>376</v>
+        <v>234</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="D50" s="27" t="s">
-        <v>375</v>
+        <v>103</v>
       </c>
       <c r="E50" s="22"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>351</v>
+        <v>257</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>352</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>354</v>
+        <v>263</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="D51" s="27" t="s">
-        <v>353</v>
+        <v>258</v>
       </c>
       <c r="E51" s="22"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B52" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D52" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="E52" s="22"/>
+    <row r="52" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B52" s="20"/>
+      <c r="C52" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D52" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="E52" s="20"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>32</v>
+        <v>166</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>357</v>
+        <v>235</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>4</v>
+        <v>170</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>77</v>
+        <v>169</v>
       </c>
       <c r="E53" s="22"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>397</v>
+        <v>370</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>483</v>
+        <v>430</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>399</v>
+        <v>372</v>
       </c>
       <c r="D54" s="27" t="s">
-        <v>398</v>
+        <v>371</v>
       </c>
       <c r="E54" s="22"/>
     </row>
-    <row r="55" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>153</v>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>347</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>325</v>
+        <v>348</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D55" s="28" t="s">
-        <v>242</v>
-      </c>
-      <c r="E55" s="18"/>
-    </row>
-    <row r="56" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>332</v>
+        <v>350</v>
+      </c>
+      <c r="D55" s="27" t="s">
+        <v>349</v>
+      </c>
+      <c r="E55" s="22"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>333</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="D56" s="28" t="s">
-        <v>335</v>
-      </c>
-      <c r="E56" s="18"/>
+        <v>265</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D56" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="E56" s="22"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B57" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E57" s="22"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="B58" s="18" t="s">
+        <v>476</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="D58" s="27" t="s">
+        <v>394</v>
+      </c>
+      <c r="E58" s="22"/>
+    </row>
+    <row r="59" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>323</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D59" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="E59" s="18"/>
+    </row>
+    <row r="60" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B60" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="D60" s="28" t="s">
+        <v>333</v>
+      </c>
+      <c r="E60" s="18"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B61" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="B57" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="C57" s="3" t="s">
+      <c r="D61" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="D57" s="27" t="s">
-        <v>224</v>
-      </c>
-      <c r="E57" s="23"/>
-    </row>
-    <row r="58" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="B58" s="18" t="s">
-        <v>260</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="D58" s="28" t="s">
-        <v>208</v>
-      </c>
-      <c r="E58" s="18"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B59" s="18" t="s">
-        <v>267</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D59" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="E59" s="22"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="B60" s="18" t="s">
-        <v>392</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="D60" s="27" t="s">
-        <v>296</v>
-      </c>
-      <c r="E60" s="22"/>
-    </row>
-    <row r="61" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B61" s="18" t="s">
-        <v>290</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D61" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="E61" s="18"/>
+      <c r="E61" s="23"/>
     </row>
     <row r="62" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>250</v>
+        <v>198</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>377</v>
+        <v>259</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D62" s="28" t="s">
-        <v>251</v>
+        <v>207</v>
       </c>
       <c r="E62" s="18"/>
     </row>
-    <row r="63" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>400</v>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B63" s="18" t="s">
-        <v>401</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="D63" s="28" t="s">
-        <v>403</v>
-      </c>
-      <c r="E63" s="18"/>
+        <v>266</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D63" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="E63" s="22"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>165</v>
+        <v>285</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>436</v>
+        <v>388</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>175</v>
+        <v>286</v>
       </c>
       <c r="D64" s="27" t="s">
-        <v>166</v>
+        <v>295</v>
       </c>
       <c r="E64" s="22"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
-        <v>35</v>
+    <row r="65" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>235</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D65" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="E65" s="22"/>
+        <v>289</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D65" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="E65" s="18"/>
     </row>
     <row r="66" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>451</v>
+        <v>373</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>84</v>
+        <v>211</v>
       </c>
       <c r="D66" s="28" t="s">
-        <v>85</v>
+        <v>250</v>
       </c>
       <c r="E66" s="18"/>
     </row>
     <row r="67" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>36</v>
+        <v>396</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>451</v>
+        <v>397</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>84</v>
+        <v>400</v>
       </c>
       <c r="D67" s="28" t="s">
-        <v>85</v>
+        <v>399</v>
       </c>
       <c r="E67" s="18"/>
     </row>
-    <row r="68" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
-        <v>254</v>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>164</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="D68" s="28" t="s">
-        <v>257</v>
-      </c>
-      <c r="E68" s="18"/>
-    </row>
-    <row r="69" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B69" s="20"/>
-      <c r="C69" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D69" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="E69" s="20"/>
+        <v>432</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D68" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="E68" s="22"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B69" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D69" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="E69" s="22"/>
     </row>
     <row r="70" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>216</v>
+        <v>237</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>126</v>
+        <v>84</v>
       </c>
       <c r="D70" s="28" t="s">
-        <v>217</v>
+        <v>85</v>
       </c>
       <c r="E70" s="18"/>
     </row>
     <row r="71" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>134</v>
+        <v>36</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>303</v>
+        <v>446</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="D71" s="28" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
       <c r="E71" s="18"/>
     </row>
     <row r="72" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>136</v>
+        <v>253</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="C72" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="D72" s="28" t="s">
+        <v>256</v>
+      </c>
+      <c r="E72" s="18"/>
+    </row>
+    <row r="73" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B73" s="20"/>
+      <c r="C73" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D72" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="E72" s="24"/>
-    </row>
-    <row r="73" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="B73" s="21" t="s">
-        <v>424</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="D73" s="28" t="s">
-        <v>300</v>
-      </c>
-      <c r="E73" s="21"/>
-    </row>
-    <row r="74" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="B74" s="20"/>
-      <c r="C74" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D74" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="E74" s="25"/>
+      <c r="D73" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="E73" s="20"/>
+    </row>
+    <row r="74" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B74" s="18" t="s">
+        <v>447</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D74" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="E74" s="18"/>
     </row>
     <row r="75" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>425</v>
+        <v>133</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>426</v>
+        <v>302</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>427</v>
+        <v>9</v>
       </c>
       <c r="D75" s="28" t="s">
-        <v>428</v>
-      </c>
-      <c r="E75" s="21"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E75" s="18"/>
+    </row>
+    <row r="76" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B76" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D76" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="E76" s="24"/>
+    </row>
+    <row r="77" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B77" s="21" t="s">
+        <v>420</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="D77" s="28" t="s">
+        <v>299</v>
+      </c>
+      <c r="E77" s="21"/>
+    </row>
+    <row r="78" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B78" s="20"/>
+      <c r="C78" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D78" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="E78" s="25"/>
+    </row>
+    <row r="79" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="B79" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="D79" s="28" t="s">
+        <v>424</v>
+      </c>
+      <c r="E79" s="21"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B76" s="18" t="s">
+      <c r="B80" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D80" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="E80" s="22"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B81" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D81" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="E81" s="22"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="B82" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D82" s="27" t="s">
+        <v>291</v>
+      </c>
+      <c r="E82" s="22"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B83" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D83" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="C76" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D76" s="27" t="s">
-        <v>243</v>
-      </c>
-      <c r="E76" s="22"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B77" s="18" t="s">
-        <v>271</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D77" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="E77" s="22"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="B78" s="18" t="s">
-        <v>326</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="D78" s="27" t="s">
-        <v>292</v>
-      </c>
-      <c r="E78" s="22"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B79" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D79" s="27" t="s">
-        <v>245</v>
-      </c>
-      <c r="E79" s="22"/>
-    </row>
-    <row r="80" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="7" t="s">
+      <c r="E83" s="22"/>
+    </row>
+    <row r="84" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B84" s="20"/>
+      <c r="C84" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D84" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="B80" s="20"/>
-      <c r="C80" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="D80" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="E80" s="20"/>
-    </row>
-    <row r="81" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B81" s="18" t="s">
-        <v>481</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D81" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="E81" s="18"/>
-    </row>
-    <row r="82" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="B82" s="18" t="s">
-        <v>267</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="D82" s="28" t="s">
-        <v>219</v>
-      </c>
-      <c r="E82" s="18"/>
-    </row>
-    <row r="83" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
-        <v>475</v>
-      </c>
-      <c r="B83" s="18" t="s">
-        <v>264</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>473</v>
-      </c>
-      <c r="D83" s="28" t="s">
-        <v>472</v>
-      </c>
-      <c r="E83" s="18"/>
-    </row>
-    <row r="84" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B84" s="18" t="s">
-        <v>263</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="D84" s="28" t="s">
-        <v>261</v>
-      </c>
-      <c r="E84" s="18"/>
+      <c r="E84" s="20"/>
     </row>
     <row r="85" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B85" s="18" t="s">
+        <v>474</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D85" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E85" s="18"/>
+    </row>
+    <row r="86" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B86" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D86" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="E86" s="18"/>
+    </row>
+    <row r="87" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="B87" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="D87" s="28" t="s">
+        <v>467</v>
+      </c>
+      <c r="E87" s="18"/>
+    </row>
+    <row r="88" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B88" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="D88" s="28" t="s">
+        <v>260</v>
+      </c>
+      <c r="E88" s="18"/>
+    </row>
+    <row r="89" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B85" s="18" t="s">
-        <v>479</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D85" s="28" t="s">
+      <c r="B89" s="18" t="s">
+        <v>485</v>
+      </c>
+      <c r="C89" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E85" s="18"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B86" s="18" t="s">
-        <v>419</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D86" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="E86" s="22"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B87" s="18" t="s">
-        <v>419</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D87" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="E87" s="22"/>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B88" s="18" t="s">
-        <v>419</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D88" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="E88" s="22"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="B89" s="18" t="s">
-        <v>443</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>444</v>
-      </c>
-      <c r="D89" s="27" t="s">
-        <v>476</v>
-      </c>
-      <c r="E89" s="22"/>
+      <c r="D89" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="E89" s="18"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>145</v>
+        <v>43</v>
       </c>
       <c r="B90" s="18" t="s">
-        <v>378</v>
+        <v>415</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="D90" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="E90" s="23"/>
-    </row>
-    <row r="91" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
-        <v>192</v>
+        <v>45</v>
+      </c>
+      <c r="E90" s="22"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="B91" s="18" t="s">
-        <v>453</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="D91" s="28" t="s">
-        <v>190</v>
-      </c>
-      <c r="E91" s="18"/>
-    </row>
-    <row r="92" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="4" t="s">
-        <v>48</v>
+        <v>415</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D91" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E91" s="22"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="B92" s="18" t="s">
-        <v>435</v>
-      </c>
-      <c r="C92" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="D92" s="28" t="s">
-        <v>320</v>
-      </c>
-      <c r="E92" s="18"/>
+        <v>415</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D92" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E92" s="22"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>202</v>
+        <v>438</v>
       </c>
       <c r="B93" s="18" t="s">
-        <v>372</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>203</v>
+        <v>439</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>440</v>
       </c>
       <c r="D93" s="27" t="s">
-        <v>204</v>
+        <v>471</v>
       </c>
       <c r="E93" s="22"/>
     </row>
-    <row r="94" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="4" t="s">
-        <v>221</v>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="B94" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="D94" s="28" t="s">
-        <v>219</v>
-      </c>
-      <c r="E94" s="18"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
-        <v>200</v>
+        <v>374</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D94" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E94" s="23"/>
+    </row>
+    <row r="95" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>191</v>
       </c>
       <c r="B95" s="18" t="s">
-        <v>280</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D95" s="27" t="s">
-        <v>201</v>
-      </c>
-      <c r="E95" s="23"/>
+        <v>448</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D95" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="E95" s="18"/>
     </row>
     <row r="96" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B96" s="18" t="s">
-        <v>339</v>
+        <v>431</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>50</v>
+        <v>319</v>
       </c>
       <c r="D96" s="28" t="s">
-        <v>86</v>
+        <v>318</v>
       </c>
       <c r="E96" s="18"/>
     </row>
-    <row r="97" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="4" t="s">
-        <v>313</v>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>201</v>
       </c>
       <c r="B97" s="18" t="s">
-        <v>454</v>
+        <v>368</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="D97" s="28" t="s">
-        <v>314</v>
-      </c>
-      <c r="E97" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="D97" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="E97" s="22"/>
     </row>
     <row r="98" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>138</v>
+        <v>220</v>
       </c>
       <c r="B98" s="18" t="s">
-        <v>312</v>
+        <v>264</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>9</v>
+        <v>217</v>
       </c>
       <c r="D98" s="28" t="s">
-        <v>139</v>
+        <v>218</v>
       </c>
       <c r="E98" s="18"/>
     </row>
-    <row r="99" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="4" t="s">
-        <v>368</v>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
+        <v>199</v>
       </c>
       <c r="B99" s="18" t="s">
-        <v>369</v>
-      </c>
-      <c r="C99" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="D99" s="28" t="s">
-        <v>371</v>
-      </c>
-      <c r="E99" s="18"/>
+        <v>279</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D99" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="E99" s="23"/>
     </row>
     <row r="100" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B100" s="18" t="s">
+        <v>494</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D100" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E100" s="18"/>
+    </row>
+    <row r="101" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="B101" s="18" t="s">
+        <v>449</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="D101" s="28" t="s">
+        <v>312</v>
+      </c>
+      <c r="E101" s="18"/>
+    </row>
+    <row r="102" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B102" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D102" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="E102" s="18"/>
+    </row>
+    <row r="103" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="B103" s="18" t="s">
+        <v>365</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="D103" s="28" t="s">
+        <v>367</v>
+      </c>
+      <c r="E103" s="18"/>
+    </row>
+    <row r="104" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B104" s="18" t="s">
+        <v>429</v>
+      </c>
+      <c r="C104" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="B100" s="18" t="s">
-        <v>433</v>
-      </c>
-      <c r="C100" s="4" t="s">
+      <c r="D104" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="D100" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="E100" s="18"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="3" t="s">
+      <c r="E104" s="18"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B101" s="18" t="s">
-        <v>310</v>
-      </c>
-      <c r="C101" s="3" t="s">
+      <c r="B105" s="18" t="s">
+        <v>308</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D105" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="E105" s="23"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B106" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="D106" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="E106" s="22"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B107" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="D107" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="E107" s="22"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="B108" s="18" t="s">
+        <v>450</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="D108" s="27" t="s">
+        <v>391</v>
+      </c>
+      <c r="E108" s="22"/>
+    </row>
+    <row r="109" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B109" s="20"/>
+      <c r="C109" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D101" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="E101" s="23"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B102" s="18" t="s">
-        <v>359</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="D102" s="27" t="s">
-        <v>273</v>
-      </c>
-      <c r="E102" s="22"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="B103" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="D103" s="27" t="s">
-        <v>230</v>
-      </c>
-      <c r="E103" s="22"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="B104" s="18" t="s">
-        <v>455</v>
-      </c>
-      <c r="C104" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="D104" s="27" t="s">
-        <v>395</v>
-      </c>
-      <c r="E104" s="22"/>
-    </row>
-    <row r="105" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="B105" s="20"/>
-      <c r="C105" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D105" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="E105" s="20"/>
-    </row>
-    <row r="106" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B106" s="18" t="s">
-        <v>429</v>
-      </c>
-      <c r="C106" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D106" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="E106" s="18"/>
-    </row>
-    <row r="107" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="B107" s="18" t="s">
-        <v>280</v>
-      </c>
-      <c r="C107" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D107" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="E107" s="18"/>
-    </row>
-    <row r="108" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="4" t="s">
-        <v>484</v>
-      </c>
-      <c r="B108" s="18" t="s">
-        <v>485</v>
-      </c>
-      <c r="C108" s="4"/>
-      <c r="D108" s="28"/>
-      <c r="E108" s="18"/>
-    </row>
-    <row r="109" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="B109" s="18" t="s">
-        <v>431</v>
-      </c>
-      <c r="C109" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D109" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="E109" s="18"/>
+      <c r="D109" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="E109" s="20"/>
     </row>
     <row r="110" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="B110" s="18" t="s">
-        <v>281</v>
+        <v>425</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>39</v>
+        <v>119</v>
       </c>
       <c r="D110" s="28" t="s">
-        <v>245</v>
+        <v>143</v>
       </c>
       <c r="E110" s="18"/>
     </row>
-    <row r="111" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="B111" s="21" t="s">
-        <v>439</v>
-      </c>
-      <c r="C111" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="D111" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="E111" s="26"/>
-    </row>
-    <row r="112" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B112" s="20"/>
-      <c r="C112" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D112" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="E112" s="25"/>
+    <row r="111" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="B111" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D111" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="E111" s="18"/>
+    </row>
+    <row r="112" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="B112" s="18" t="s">
+        <v>478</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="D112" s="28" t="s">
+        <v>483</v>
+      </c>
+      <c r="E112" s="18"/>
     </row>
     <row r="113" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
-        <v>381</v>
+        <v>426</v>
       </c>
       <c r="B113" s="18" t="s">
+        <v>427</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D113" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="E113" s="18"/>
+    </row>
+    <row r="114" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B114" s="21" t="s">
+        <v>435</v>
+      </c>
+      <c r="C114" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="C113" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="D113" s="28" t="s">
-        <v>382</v>
-      </c>
-      <c r="E113" s="21"/>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B114" s="18" t="s">
-        <v>346</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>121</v>
-      </c>
       <c r="D114" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="E114" s="22"/>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B115" s="18" t="s">
-        <v>346</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D115" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="E115" s="22"/>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="3" t="s">
-        <v>58</v>
+        <v>149</v>
+      </c>
+      <c r="E114" s="26"/>
+    </row>
+    <row r="115" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B115" s="20"/>
+      <c r="C115" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D115" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="E115" s="25"/>
+    </row>
+    <row r="116" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
+        <v>377</v>
       </c>
       <c r="B116" s="18" t="s">
-        <v>346</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D116" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="E116" s="22"/>
+        <v>147</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="D116" s="28" t="s">
+        <v>378</v>
+      </c>
+      <c r="E116" s="21"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B117" s="18" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C117" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D117" s="27" t="s">
         <v>121</v>
-      </c>
-      <c r="D117" s="27" t="s">
-        <v>122</v>
       </c>
       <c r="E117" s="22"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B118" s="18" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C118" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D118" s="27" t="s">
         <v>121</v>
-      </c>
-      <c r="D118" s="27" t="s">
-        <v>122</v>
       </c>
       <c r="E118" s="22"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
-        <v>284</v>
+        <v>58</v>
       </c>
       <c r="B119" s="18" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>283</v>
+        <v>120</v>
       </c>
       <c r="D119" s="27" t="s">
-        <v>282</v>
+        <v>121</v>
       </c>
       <c r="E119" s="22"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
-        <v>336</v>
+        <v>59</v>
       </c>
       <c r="B120" s="18" t="s">
-        <v>324</v>
+        <v>342</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>338</v>
+        <v>120</v>
       </c>
       <c r="D120" s="27" t="s">
-        <v>337</v>
+        <v>121</v>
       </c>
       <c r="E120" s="22"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B121" s="18" t="s">
-        <v>237</v>
+        <v>342</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>29</v>
+        <v>120</v>
       </c>
       <c r="D121" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E121" s="22"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>62</v>
+        <v>283</v>
       </c>
       <c r="B122" s="18" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>124</v>
+        <v>282</v>
       </c>
       <c r="D122" s="27" t="s">
-        <v>247</v>
-      </c>
-      <c r="E122" s="23"/>
+        <v>281</v>
+      </c>
+      <c r="E122" s="22"/>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
-        <v>305</v>
+        <v>334</v>
       </c>
       <c r="B123" s="18" t="s">
-        <v>480</v>
+        <v>322</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>309</v>
+        <v>336</v>
       </c>
       <c r="D123" s="27" t="s">
-        <v>308</v>
-      </c>
-      <c r="E123" s="23"/>
-    </row>
-    <row r="124" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="4" t="s">
-        <v>63</v>
+        <v>335</v>
+      </c>
+      <c r="E123" s="22"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="B124" s="18" t="s">
-        <v>350</v>
-      </c>
-      <c r="C124" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D124" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="E124" s="18"/>
+        <v>236</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D124" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="E124" s="22"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
-        <v>183</v>
+        <v>62</v>
       </c>
       <c r="B125" s="18" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>184</v>
+        <v>123</v>
       </c>
       <c r="D125" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="E125" s="22"/>
-    </row>
-    <row r="126" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="4" t="s">
-        <v>207</v>
+        <v>246</v>
+      </c>
+      <c r="E125" s="23"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
+        <v>303</v>
       </c>
       <c r="B126" s="18" t="s">
-        <v>379</v>
-      </c>
-      <c r="C126" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D126" s="28" t="s">
-        <v>206</v>
-      </c>
-      <c r="E126" s="18"/>
+        <v>473</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D126" s="27" t="s">
+        <v>306</v>
+      </c>
+      <c r="E126" s="23"/>
     </row>
     <row r="127" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
-        <v>268</v>
+        <v>63</v>
       </c>
       <c r="B127" s="18" t="s">
-        <v>269</v>
+        <v>346</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>175</v>
+        <v>64</v>
       </c>
       <c r="D127" s="28" t="s">
-        <v>270</v>
+        <v>83</v>
       </c>
       <c r="E127" s="18"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="B128" s="18" t="s">
-        <v>275</v>
+        <v>338</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>164</v>
+        <v>183</v>
       </c>
       <c r="D128" s="27" t="s">
-        <v>163</v>
+        <v>184</v>
       </c>
       <c r="E128" s="22"/>
     </row>
     <row r="129" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
-        <v>465</v>
-      </c>
-      <c r="B129" s="18"/>
+        <v>206</v>
+      </c>
+      <c r="B129" s="18" t="s">
+        <v>375</v>
+      </c>
       <c r="C129" s="4" t="s">
-        <v>467</v>
+        <v>26</v>
       </c>
       <c r="D129" s="28" t="s">
-        <v>466</v>
+        <v>205</v>
       </c>
       <c r="E129" s="18"/>
     </row>
     <row r="130" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
-        <v>195</v>
+        <v>267</v>
       </c>
       <c r="B130" s="18" t="s">
-        <v>432</v>
+        <v>268</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="D130" s="28" t="s">
-        <v>194</v>
+        <v>269</v>
       </c>
       <c r="E130" s="18"/>
     </row>
-    <row r="131" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B131" s="21" t="s">
-        <v>409</v>
-      </c>
-      <c r="C131" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="D131" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="E131" s="21"/>
-      <c r="F131" s="16"/>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B131" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D131" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="E131" s="22"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="B132" s="18" t="s">
+        <v>501</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="D132" s="27" t="s">
+        <v>500</v>
+      </c>
+      <c r="E132" s="22"/>
+    </row>
+    <row r="133" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="B133" s="18" t="s">
+        <v>503</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="D133" s="28" t="s">
+        <v>461</v>
+      </c>
+      <c r="E133" s="18"/>
+    </row>
+    <row r="134" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B134" s="18" t="s">
+        <v>428</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D134" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="E134" s="18"/>
+    </row>
+    <row r="135" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B135" s="21" t="s">
+        <v>405</v>
+      </c>
+      <c r="C135" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D135" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="E135" s="21"/>
+      <c r="F135" s="16"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B132" s="18" t="s">
-        <v>288</v>
-      </c>
-      <c r="C132" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D132" s="27" t="s">
+      <c r="B136" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="C136" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E132" s="22"/>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A133" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B133" s="18" t="s">
-        <v>240</v>
-      </c>
-      <c r="C133" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D133" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="E133" s="22"/>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="B134" s="18" t="s">
-        <v>297</v>
-      </c>
-      <c r="C134" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D134" s="27" t="s">
-        <v>253</v>
-      </c>
-      <c r="E134" s="22"/>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" s="3" t="s">
-        <v>469</v>
-      </c>
-      <c r="B135" s="18" t="s">
-        <v>267</v>
-      </c>
-      <c r="C135" s="3" t="s">
-        <v>470</v>
-      </c>
-      <c r="D135" s="27" t="s">
-        <v>468</v>
-      </c>
-      <c r="E135" s="22"/>
-    </row>
-    <row r="136" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B136" s="18" t="s">
-        <v>248</v>
-      </c>
-      <c r="C136" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D136" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="E136" s="18"/>
+      <c r="D136" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="E136" s="22"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
-        <v>66</v>
+        <v>158</v>
       </c>
       <c r="B137" s="18" t="s">
-        <v>446</v>
+        <v>239</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>53</v>
+        <v>125</v>
       </c>
       <c r="D137" s="27" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="E137" s="22"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>457</v>
+        <v>251</v>
       </c>
       <c r="B138" s="18" t="s">
-        <v>460</v>
+        <v>296</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>459</v>
+        <v>125</v>
       </c>
       <c r="D138" s="27" t="s">
-        <v>458</v>
+        <v>252</v>
       </c>
       <c r="E138" s="22"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
-        <v>71</v>
+        <v>464</v>
       </c>
       <c r="B139" s="18" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>53</v>
+        <v>465</v>
       </c>
       <c r="D139" s="27" t="s">
-        <v>127</v>
+        <v>463</v>
       </c>
       <c r="E139" s="22"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A140" s="3" t="s">
-        <v>67</v>
+    <row r="140" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="B140" s="18" t="s">
-        <v>456</v>
-      </c>
-      <c r="C140" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D140" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="E140" s="23"/>
+        <v>247</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D140" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E140" s="18"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
-        <v>405</v>
+        <v>66</v>
       </c>
       <c r="B141" s="18" t="s">
-        <v>408</v>
-      </c>
-      <c r="C141" s="4" t="s">
-        <v>407</v>
+        <v>442</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="D141" s="27" t="s">
-        <v>406</v>
-      </c>
-      <c r="E141" s="23"/>
+        <v>126</v>
+      </c>
+      <c r="E141" s="22"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
-        <v>386</v>
+        <v>452</v>
       </c>
       <c r="B142" s="18" t="s">
-        <v>387</v>
-      </c>
-      <c r="C142" s="4" t="s">
-        <v>388</v>
+        <v>455</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>454</v>
       </c>
       <c r="D142" s="27" t="s">
-        <v>389</v>
-      </c>
-      <c r="E142" s="23"/>
-    </row>
-    <row r="143" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="B143" s="20"/>
-      <c r="C143" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="D143" s="30" t="s">
-        <v>211</v>
-      </c>
-      <c r="E143" s="20"/>
+        <v>453</v>
+      </c>
+      <c r="E142" s="22"/>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B143" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D143" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="E143" s="22"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B144" s="18" t="s">
-        <v>385</v>
+        <v>451</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>161</v>
+        <v>68</v>
       </c>
       <c r="D144" s="27" t="s">
-        <v>129</v>
-      </c>
-      <c r="E144" s="22"/>
-    </row>
-    <row r="145" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="4" t="s">
-        <v>70</v>
+        <v>127</v>
+      </c>
+      <c r="E144" s="23"/>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="3" t="s">
+        <v>401</v>
       </c>
       <c r="B145" s="18" t="s">
-        <v>384</v>
+        <v>404</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D145" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="E145" s="18"/>
+        <v>403</v>
+      </c>
+      <c r="D145" s="27" t="s">
+        <v>402</v>
+      </c>
+      <c r="E145" s="23"/>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="B146" s="15" t="s">
-        <v>415</v>
+        <v>382</v>
+      </c>
+      <c r="B146" s="18" t="s">
+        <v>383</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D146" s="28" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B147" s="18" t="s">
-        <v>358</v>
-      </c>
-      <c r="C147" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D147" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="E147" s="18"/>
+        <v>384</v>
+      </c>
+      <c r="D146" s="27" t="s">
+        <v>385</v>
+      </c>
+      <c r="E146" s="23"/>
+    </row>
+    <row r="147" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B147" s="20"/>
+      <c r="C147" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D147" s="30" t="s">
+        <v>210</v>
+      </c>
+      <c r="E147" s="20"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B148" s="18" t="s">
-        <v>327</v>
+        <v>381</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="D148" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="E148" s="23"/>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A149" s="3" t="s">
-        <v>74</v>
+        <v>128</v>
+      </c>
+      <c r="E148" s="22"/>
+    </row>
+    <row r="149" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="B149" s="18" t="s">
-        <v>298</v>
-      </c>
-      <c r="C149" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D149" s="27" t="s">
-        <v>245</v>
-      </c>
-      <c r="E149" s="22"/>
+        <v>380</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D149" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="E149" s="18"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B150" s="18" t="s">
-        <v>391</v>
-      </c>
-      <c r="C150" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D150" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="E150" s="23"/>
+        <v>226</v>
+      </c>
+      <c r="B150" s="15" t="s">
+        <v>411</v>
+      </c>
+      <c r="C150" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D150" s="28" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="151" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B151" s="18" t="s">
-        <v>328</v>
+        <v>354</v>
       </c>
       <c r="C151" s="4" t="s">
         <v>4</v>
@@ -4246,95 +4303,171 @@
       </c>
       <c r="E151" s="18"/>
     </row>
-    <row r="152" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="4" t="s">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B152" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D152" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="E152" s="23"/>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B153" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D153" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="E153" s="22"/>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B154" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D154" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="E154" s="23"/>
+    </row>
+    <row r="155" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B155" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="C155" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D155" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="E155" s="18"/>
+    </row>
+    <row r="156" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B156" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="C156" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B152" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="C152" s="4" t="s">
+      <c r="D156" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="D152" s="28" t="s">
-        <v>215</v>
-      </c>
-      <c r="E152" s="18"/>
+      <c r="E156" s="18"/>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="B157" s="15" t="s">
+        <v>482</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="D157" s="27" t="s">
+        <v>480</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D85" r:id="rId1"/>
-    <hyperlink ref="D151" r:id="rId2"/>
-    <hyperlink ref="D150" r:id="rId3"/>
-    <hyperlink ref="D148" r:id="rId4"/>
-    <hyperlink ref="D147" r:id="rId5"/>
-    <hyperlink ref="D139" r:id="rId6"/>
-    <hyperlink ref="D145" r:id="rId7"/>
-    <hyperlink ref="D144" r:id="rId8"/>
-    <hyperlink ref="D140" r:id="rId9"/>
-    <hyperlink ref="D137" r:id="rId10"/>
-    <hyperlink ref="D136" r:id="rId11"/>
-    <hyperlink ref="D132" r:id="rId12"/>
-    <hyperlink ref="D77" r:id="rId13"/>
-    <hyperlink ref="D124" r:id="rId14"/>
-    <hyperlink ref="D118" r:id="rId15"/>
-    <hyperlink ref="D74" r:id="rId16"/>
-    <hyperlink ref="D72" r:id="rId17"/>
-    <hyperlink ref="D71" r:id="rId18"/>
-    <hyperlink ref="D69" r:id="rId19"/>
-    <hyperlink ref="D67" r:id="rId20"/>
-    <hyperlink ref="D65" r:id="rId21"/>
-    <hyperlink ref="D66" r:id="rId22"/>
-    <hyperlink ref="D61" r:id="rId23"/>
-    <hyperlink ref="D59" r:id="rId24"/>
-    <hyperlink ref="D53" r:id="rId25"/>
-    <hyperlink ref="D46" r:id="rId26"/>
-    <hyperlink ref="D43" r:id="rId27"/>
-    <hyperlink ref="D41" r:id="rId28"/>
-    <hyperlink ref="D37" r:id="rId29"/>
-    <hyperlink ref="D36" r:id="rId30"/>
-    <hyperlink ref="D33" r:id="rId31"/>
-    <hyperlink ref="D32" r:id="rId32"/>
-    <hyperlink ref="D31" r:id="rId33"/>
-    <hyperlink ref="D29" r:id="rId34"/>
-    <hyperlink ref="D28" r:id="rId35"/>
-    <hyperlink ref="D27" r:id="rId36"/>
-    <hyperlink ref="D26" r:id="rId37"/>
-    <hyperlink ref="D22" r:id="rId38"/>
+    <hyperlink ref="D89" r:id="rId1"/>
+    <hyperlink ref="D155" r:id="rId2"/>
+    <hyperlink ref="D154" r:id="rId3"/>
+    <hyperlink ref="D152" r:id="rId4"/>
+    <hyperlink ref="D151" r:id="rId5"/>
+    <hyperlink ref="D143" r:id="rId6"/>
+    <hyperlink ref="D149" r:id="rId7"/>
+    <hyperlink ref="D148" r:id="rId8"/>
+    <hyperlink ref="D144" r:id="rId9"/>
+    <hyperlink ref="D141" r:id="rId10"/>
+    <hyperlink ref="D140" r:id="rId11"/>
+    <hyperlink ref="D136" r:id="rId12"/>
+    <hyperlink ref="D81" r:id="rId13"/>
+    <hyperlink ref="D127" r:id="rId14"/>
+    <hyperlink ref="D121" r:id="rId15"/>
+    <hyperlink ref="D78" r:id="rId16"/>
+    <hyperlink ref="D76" r:id="rId17"/>
+    <hyperlink ref="D75" r:id="rId18"/>
+    <hyperlink ref="D73" r:id="rId19"/>
+    <hyperlink ref="D71" r:id="rId20"/>
+    <hyperlink ref="D69" r:id="rId21"/>
+    <hyperlink ref="D70" r:id="rId22"/>
+    <hyperlink ref="D65" r:id="rId23"/>
+    <hyperlink ref="D63" r:id="rId24"/>
+    <hyperlink ref="D57" r:id="rId25"/>
+    <hyperlink ref="D50" r:id="rId26"/>
+    <hyperlink ref="D47" r:id="rId27"/>
+    <hyperlink ref="D45" r:id="rId28"/>
+    <hyperlink ref="D41" r:id="rId29"/>
+    <hyperlink ref="D40" r:id="rId30"/>
+    <hyperlink ref="D37" r:id="rId31"/>
+    <hyperlink ref="D36" r:id="rId32"/>
+    <hyperlink ref="D35" r:id="rId33"/>
+    <hyperlink ref="D33" r:id="rId34"/>
+    <hyperlink ref="D32" r:id="rId35"/>
+    <hyperlink ref="D31" r:id="rId36"/>
+    <hyperlink ref="D30" r:id="rId37"/>
+    <hyperlink ref="D26" r:id="rId38"/>
     <hyperlink ref="D6" r:id="rId39"/>
     <hyperlink ref="D15" r:id="rId40"/>
     <hyperlink ref="D9" r:id="rId41"/>
     <hyperlink ref="D4" r:id="rId42"/>
     <hyperlink ref="D3" r:id="rId43"/>
     <hyperlink ref="D2" r:id="rId44"/>
-    <hyperlink ref="D87" r:id="rId45"/>
-    <hyperlink ref="D117" r:id="rId46"/>
-    <hyperlink ref="D116" r:id="rId47"/>
-    <hyperlink ref="D115" r:id="rId48"/>
-    <hyperlink ref="D114" r:id="rId49"/>
-    <hyperlink ref="D112" r:id="rId50"/>
-    <hyperlink ref="D111" r:id="rId51"/>
-    <hyperlink ref="D98" r:id="rId52"/>
-    <hyperlink ref="D96" r:id="rId53"/>
-    <hyperlink ref="D90" r:id="rId54"/>
-    <hyperlink ref="D88" r:id="rId55"/>
+    <hyperlink ref="D91" r:id="rId45"/>
+    <hyperlink ref="D120" r:id="rId46"/>
+    <hyperlink ref="D119" r:id="rId47"/>
+    <hyperlink ref="D118" r:id="rId48"/>
+    <hyperlink ref="D117" r:id="rId49"/>
+    <hyperlink ref="D115" r:id="rId50"/>
+    <hyperlink ref="D114" r:id="rId51"/>
+    <hyperlink ref="D102" r:id="rId52"/>
+    <hyperlink ref="D100" r:id="rId53"/>
+    <hyperlink ref="D94" r:id="rId54"/>
+    <hyperlink ref="D92" r:id="rId55"/>
     <hyperlink ref="D16" r:id="rId56"/>
-    <hyperlink ref="D152" r:id="rId57"/>
+    <hyperlink ref="D156" r:id="rId57"/>
     <hyperlink ref="D7" r:id="rId58"/>
     <hyperlink ref="D5" r:id="rId59"/>
     <hyperlink ref="D10" r:id="rId60"/>
-    <hyperlink ref="D146" r:id="rId61"/>
-    <hyperlink ref="D76" r:id="rId62"/>
-    <hyperlink ref="D121" r:id="rId63"/>
-    <hyperlink ref="D44" r:id="rId64"/>
-    <hyperlink ref="D78" r:id="rId65"/>
-    <hyperlink ref="D24" r:id="rId66"/>
+    <hyperlink ref="D150" r:id="rId61"/>
+    <hyperlink ref="D80" r:id="rId62"/>
+    <hyperlink ref="D124" r:id="rId63"/>
+    <hyperlink ref="D48" r:id="rId64"/>
+    <hyperlink ref="D82" r:id="rId65"/>
+    <hyperlink ref="D28" r:id="rId66"/>
     <hyperlink ref="D8" r:id="rId67"/>
-    <hyperlink ref="D86" r:id="rId68"/>
-    <hyperlink ref="D34" r:id="rId69"/>
+    <hyperlink ref="D90" r:id="rId68"/>
+    <hyperlink ref="D38" r:id="rId69"/>
+    <hyperlink ref="D157" r:id="rId70"/>
+    <hyperlink ref="D24" r:id="rId71"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId70"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId72"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updates, Script progress and bug fixes
</commit_message>
<xml_diff>
--- a/Modlist.xlsx
+++ b/Modlist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="520">
   <si>
     <t>Mod</t>
   </si>
@@ -111,9 +111,6 @@
     <t>URL</t>
   </si>
   <si>
-    <t>Damage Indicators</t>
-  </si>
-  <si>
     <t>Ender Storage</t>
   </si>
   <si>
@@ -327,12 +324,6 @@
     <t>http://computercraft.info/wiki/Main_Page</t>
   </si>
   <si>
-    <t>http://www.minecraftforum.net/topic/1536685-172164forge-hit-splat-damage-indicators-v304-rpg-ui-and-damage-amount-mod/</t>
-  </si>
-  <si>
-    <t>Rich1051414</t>
-  </si>
-  <si>
     <t>http://www.minecraftforum.net/topic/1776056-164forge-extra-utilities-v102/</t>
   </si>
   <si>
@@ -561,9 +552,6 @@
     <t>http://www.minecraftforum.net/topic/2319703-aobd-ticic2eiomekanism-add-on-process-cobalt-ardite-and-aluminium-v140/</t>
   </si>
   <si>
-    <t>Planetguy</t>
-  </si>
-  <si>
     <t>Better Dungeons</t>
   </si>
   <si>
@@ -624,12 +612,6 @@
     <t>Resonant Engine</t>
   </si>
   <si>
-    <t>http://calclavia.com/resonant-induction/</t>
-  </si>
-  <si>
-    <t>Resonant Induction Core</t>
-  </si>
-  <si>
     <t>http://www.minecraftforum.net/topic/1985397-forge-extratic-tinkers-construct-mod-support-add-on/</t>
   </si>
   <si>
@@ -648,12 +630,6 @@
     <t>Xeno's Reliquary</t>
   </si>
   <si>
-    <t>TheMike</t>
-  </si>
-  <si>
-    <t>http://www.minecraftforum.net/topic/2237899-164v112-reliquary/</t>
-  </si>
-  <si>
     <t>Hardcore Questing Mode</t>
   </si>
   <si>
@@ -711,9 +687,6 @@
     <t>1.12.0.4</t>
   </si>
   <si>
-    <t>3.2.0</t>
-  </si>
-  <si>
     <t>r38</t>
   </si>
   <si>
@@ -945,12 +918,6 @@
     <t>Chisel 2</t>
   </si>
   <si>
-    <t>PlanetGuyLib</t>
-  </si>
-  <si>
-    <t>https://www.mediafire.com/folder/nx48d9udpfpln/RemainInMotion#m1098max26eqc</t>
-  </si>
-  <si>
     <t>https://jakimfett.github.io/Minechem/</t>
   </si>
   <si>
@@ -966,9 +933,6 @@
     <t>1.5</t>
   </si>
   <si>
-    <t>1.0.0B7-19</t>
-  </si>
-  <si>
     <t>2.3.2</t>
   </si>
   <si>
@@ -1041,9 +1005,6 @@
     <t>Chisel Facades</t>
   </si>
   <si>
-    <t>0.4.0A</t>
-  </si>
-  <si>
     <t>http://minecraft.curseforge.com/mc-mods/225280-chococraft</t>
   </si>
   <si>
@@ -1068,9 +1029,6 @@
     <t>3.0.9c</t>
   </si>
   <si>
-    <t>1.65</t>
-  </si>
-  <si>
     <t>Ender IO</t>
   </si>
   <si>
@@ -1083,9 +1041,6 @@
     <t>4.1.1.59</t>
   </si>
   <si>
-    <t>0.3.5.257</t>
-  </si>
-  <si>
     <t>3.0.0.363</t>
   </si>
   <si>
@@ -1176,9 +1131,6 @@
     <t>MCCommander_Minecraft</t>
   </si>
   <si>
-    <t>7.1.1.145</t>
-  </si>
-  <si>
     <t>Ancient Warfare</t>
   </si>
   <si>
@@ -1224,9 +1176,6 @@
     <t>5.0.5.348</t>
   </si>
   <si>
-    <t>0.552</t>
-  </si>
-  <si>
     <t>http://www.minecraftforum.net/forums/mapping-and-modding/minecraft-mods/2310397-additional-buildcraft-objects-a-plugin-for</t>
   </si>
   <si>
@@ -1257,12 +1206,6 @@
     <t>1.8.2a</t>
   </si>
   <si>
-    <t>6.3.1</t>
-  </si>
-  <si>
-    <t>1.3.0b-3</t>
-  </si>
-  <si>
     <t>3.0.6.254</t>
   </si>
   <si>
@@ -1335,9 +1278,6 @@
     <t>a-1.3.0.1</t>
   </si>
   <si>
-    <t>0.8.3.91</t>
-  </si>
-  <si>
     <t>3.0.10</t>
   </si>
   <si>
@@ -1413,9 +1353,6 @@
     <t>2.4.0</t>
   </si>
   <si>
-    <t>4.2.3.4</t>
-  </si>
-  <si>
     <t>3.3.5</t>
   </si>
   <si>
@@ -1431,18 +1368,12 @@
     <t>0.2a</t>
   </si>
   <si>
-    <t>1.2.2</t>
-  </si>
-  <si>
     <t>1.19</t>
   </si>
   <si>
     <t>1.17</t>
   </si>
   <si>
-    <t>1.4b3</t>
-  </si>
-  <si>
     <t>0.9.8bf1</t>
   </si>
   <si>
@@ -1524,33 +1455,15 @@
     <t>1.2.1</t>
   </si>
   <si>
-    <t>3.0.0RC1-186</t>
-  </si>
-  <si>
-    <t>1.0.0B9-113</t>
-  </si>
-  <si>
     <t>ChiselTones</t>
   </si>
   <si>
     <t>http://minecraft.curseforge.com/mc-mods/228004-chiseltones</t>
   </si>
   <si>
-    <t>6.3.7</t>
-  </si>
-  <si>
-    <t>4.0.0RC1-120</t>
-  </si>
-  <si>
-    <t>1.0.0RC2-54</t>
-  </si>
-  <si>
     <t>Thermal Dynamics</t>
   </si>
   <si>
-    <t>1.0.0RC1-69</t>
-  </si>
-  <si>
     <t>1.1.0RC2-43</t>
   </si>
   <si>
@@ -1569,12 +1482,6 @@
     <t>TehNut</t>
   </si>
   <si>
-    <t>1.3.0-a4-b358</t>
-  </si>
-  <si>
-    <t>4.5.12.64</t>
-  </si>
-  <si>
     <t>Funky Locomotion</t>
   </si>
   <si>
@@ -1584,10 +1491,91 @@
     <t>http://minecraft.curseforge.com/mc-mods/224190-funky-locomotion</t>
   </si>
   <si>
-    <t>0.7</t>
-  </si>
-  <si>
     <t>Joshie, Jared</t>
+  </si>
+  <si>
+    <t>3.0.0RC2-196</t>
+  </si>
+  <si>
+    <t>1.0.0B9-118</t>
+  </si>
+  <si>
+    <t>0.4.2A</t>
+  </si>
+  <si>
+    <t>0.7.1</t>
+  </si>
+  <si>
+    <t>4.0.0RC2-129</t>
+  </si>
+  <si>
+    <t>1.0.0RC3-56</t>
+  </si>
+  <si>
+    <t>1.0.0RC2-77</t>
+  </si>
+  <si>
+    <t>3.966</t>
+  </si>
+  <si>
+    <t>Thaumic Horizons</t>
+  </si>
+  <si>
+    <t>http://minecraft.curseforge.com/mc-mods/227914-thaumic-horizons</t>
+  </si>
+  <si>
+    <t>Kentington</t>
+  </si>
+  <si>
+    <t>1.3.0-a5-b365</t>
+  </si>
+  <si>
+    <t>4.2.3.5</t>
+  </si>
+  <si>
+    <t>http://www.minecraftforum.net/forums/mapping-and-modding/minecraft-mods/2234220-xenos-reliquary</t>
+  </si>
+  <si>
+    <t>x3n0ph0b3</t>
+  </si>
+  <si>
+    <t>7.1.2.177</t>
+  </si>
+  <si>
+    <t>GardenStuff</t>
+  </si>
+  <si>
+    <t>http://minecraft.curseforge.com/mc-mods/225903-garden-stuff</t>
+  </si>
+  <si>
+    <t>1.73</t>
+  </si>
+  <si>
+    <t>0.561</t>
+  </si>
+  <si>
+    <t>0.8.3.104</t>
+  </si>
+  <si>
+    <t>1.0.0B9-54</t>
+  </si>
+  <si>
+    <t>6.4.1</t>
+  </si>
+  <si>
+    <t>6.4.0</t>
+  </si>
+  <si>
+    <t>1.3.1-2</t>
+  </si>
+  <si>
+    <t>4.5.13.65</t>
+  </si>
+  <si>
+    <t>1.3.2</t>
+  </si>
+  <si>
+    <t>1.4c</t>
   </si>
 </sst>
 </file>
@@ -1784,7 +1772,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1823,8 +1811,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2127,17 +2119,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F163"/>
+  <dimension ref="A1:F162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C104" sqref="C104"/>
+      <selection pane="bottomLeft" activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.42578125" style="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="40" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="166.85546875" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="15" hidden="1" customWidth="1"/>
@@ -2150,7 +2142,7 @@
       <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="39" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -2160,21 +2152,21 @@
         <v>30</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="33" t="s">
-        <v>485</v>
+      <c r="B2" s="40" t="s">
+        <v>462</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E2" s="21"/>
     </row>
@@ -2182,14 +2174,14 @@
       <c r="A3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="34" t="s">
-        <v>486</v>
+      <c r="B3" s="38" t="s">
+        <v>463</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3" s="18"/>
     </row>
@@ -2197,44 +2189,44 @@
       <c r="A4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="34" t="s">
-        <v>230</v>
+      <c r="B4" s="38" t="s">
+        <v>222</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
-        <v>222</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>338</v>
+        <v>214</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>326</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E5" s="22"/>
     </row>
     <row r="6" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="B6" s="34" t="s">
-        <v>356</v>
+        <v>197</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>341</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E6" s="18"/>
     </row>
@@ -2242,43 +2234,43 @@
       <c r="A7" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="34" t="s">
-        <v>502</v>
+      <c r="B7" s="38" t="s">
+        <v>492</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
-        <v>384</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>503</v>
+        <v>369</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>493</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="34" t="s">
-        <v>415</v>
+      <c r="B9" s="38" t="s">
+        <v>396</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="29" t="s">
         <v>84</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>85</v>
       </c>
       <c r="E9" s="18"/>
     </row>
@@ -2286,1216 +2278,1216 @@
       <c r="A10" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="34" t="s">
-        <v>244</v>
+      <c r="B10" s="38" t="s">
+        <v>235</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>274</v>
+        <v>139</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>265</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>275</v>
+        <v>98</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>266</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>292</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>329</v>
+        <v>283</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>317</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="E13" s="18"/>
     </row>
-    <row r="14" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>309</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>233</v>
+        <v>12</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>464</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>181</v>
+        <v>49</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>310</v>
+        <v>85</v>
       </c>
       <c r="E14" s="18"/>
     </row>
     <row r="15" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="34" t="s">
-        <v>487</v>
+        <v>435</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>436</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>50</v>
+        <v>441</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" s="18"/>
+        <v>443</v>
+      </c>
     </row>
     <row r="16" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>455</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>456</v>
+        <v>437</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>406</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>461</v>
+        <v>441</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>463</v>
+        <v>442</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>457</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>425</v>
+        <v>316</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>317</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>461</v>
+        <v>315</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>462</v>
+        <v>318</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>328</v>
-      </c>
-      <c r="B18" s="34" t="s">
-        <v>329</v>
+        <v>413</v>
+      </c>
+      <c r="B18" s="38" t="s">
+        <v>416</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>330</v>
+        <v>415</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>432</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>435</v>
+        <v>460</v>
+      </c>
+      <c r="B19" s="38" t="s">
+        <v>226</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>433</v>
+        <v>370</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B20" s="34" t="s">
-        <v>235</v>
+        <v>467</v>
+      </c>
+      <c r="B20" s="38" t="s">
+        <v>468</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>385</v>
-      </c>
-      <c r="D20" s="29" t="s">
-        <v>305</v>
+        <v>441</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="B21" s="34" t="s">
-        <v>491</v>
+        <v>469</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>402</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>461</v>
+        <v>441</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>459</v>
+        <v>439</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="B22" s="34" t="s">
-        <v>421</v>
+        <v>470</v>
+      </c>
+      <c r="B22" s="38" t="s">
+        <v>473</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>461</v>
-      </c>
-      <c r="D22" s="28" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>493</v>
-      </c>
-      <c r="B23" s="34" t="s">
-        <v>496</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>495</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="38"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="27"/>
+        <v>472</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="41"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="27"/>
+    </row>
+    <row r="24" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="B24" s="38" t="s">
+        <v>503</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>290</v>
+      </c>
+      <c r="E24" s="18"/>
     </row>
     <row r="25" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="B25" s="34" t="s">
-        <v>517</v>
+        <v>371</v>
+      </c>
+      <c r="B25" s="38" t="s">
+        <v>372</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>271</v>
+        <v>374</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>299</v>
+        <v>373</v>
       </c>
       <c r="E25" s="18"/>
     </row>
     <row r="26" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>387</v>
-      </c>
-      <c r="B26" s="34" t="s">
-        <v>388</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>390</v>
+        <v>430</v>
+      </c>
+      <c r="B26" s="38" t="s">
+        <v>433</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>431</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>389</v>
+        <v>432</v>
       </c>
       <c r="E26" s="18"/>
     </row>
-    <row r="27" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
-        <v>450</v>
-      </c>
-      <c r="B27" s="34" t="s">
-        <v>453</v>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="B27" s="38" t="s">
+        <v>444</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>451</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>452</v>
-      </c>
-      <c r="E27" s="18"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="33" t="s">
-        <v>178</v>
-      </c>
-      <c r="B28" s="34" t="s">
-        <v>464</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D28" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="E28" s="21"/>
+        <v>176</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="E27" s="21"/>
+    </row>
+    <row r="28" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="38" t="s">
+        <v>459</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" s="20"/>
     </row>
     <row r="29" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="34" t="s">
-        <v>482</v>
+        <v>365</v>
+      </c>
+      <c r="B29" s="38" t="s">
+        <v>366</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>25</v>
+        <v>368</v>
       </c>
       <c r="D29" s="29" t="s">
+        <v>367</v>
+      </c>
+      <c r="E29" s="20"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="B30" s="38" t="s">
+        <v>429</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="E29" s="20"/>
-    </row>
-    <row r="30" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
-        <v>380</v>
-      </c>
-      <c r="B30" s="34" t="s">
-        <v>381</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="D30" s="29" t="s">
-        <v>382</v>
-      </c>
-      <c r="E30" s="20"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="B31" s="34" t="s">
-        <v>449</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D31" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="E31" s="21"/>
-    </row>
-    <row r="32" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="34" t="s">
-        <v>182</v>
-      </c>
-      <c r="B32" s="34" t="s">
-        <v>279</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="D32" s="29" t="s">
-        <v>184</v>
-      </c>
-      <c r="E32" s="18"/>
+      <c r="E30" s="21"/>
+    </row>
+    <row r="31" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="B31" s="38" t="s">
+        <v>270</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="E31" s="18"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="38" t="s">
+        <v>302</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" s="21"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="34" t="s">
-        <v>313</v>
+        <v>15</v>
+      </c>
+      <c r="B33" s="38" t="s">
+        <v>280</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E33" s="21"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="B34" s="34" t="s">
-        <v>289</v>
+        <v>16</v>
+      </c>
+      <c r="B34" s="38" t="s">
+        <v>303</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D34" s="28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E34" s="21"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" s="34" t="s">
-        <v>314</v>
+        <v>17</v>
+      </c>
+      <c r="B35" s="38" t="s">
+        <v>304</v>
       </c>
       <c r="C35" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="E35" s="21"/>
+    </row>
+    <row r="36" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="34" t="s">
+        <v>188</v>
+      </c>
+      <c r="B36" s="38" t="s">
+        <v>494</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="E36" s="18"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="38" t="s">
+        <v>331</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="D35" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="E35" s="21"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="B36" s="34" t="s">
-        <v>315</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D36" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="E36" s="21"/>
-    </row>
-    <row r="37" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="34" t="s">
-        <v>192</v>
-      </c>
-      <c r="B37" s="34" t="s">
-        <v>341</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="D37" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="E37" s="18"/>
+      <c r="E37" s="21"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38" s="34" t="s">
-        <v>344</v>
+        <v>19</v>
+      </c>
+      <c r="B38" s="38" t="s">
+        <v>516</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>94</v>
       </c>
       <c r="D38" s="28" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E38" s="21"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" s="34" t="s">
-        <v>414</v>
+        <v>20</v>
+      </c>
+      <c r="B39" s="38" t="s">
+        <v>514</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>95</v>
+        <v>279</v>
       </c>
       <c r="D39" s="28" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E39" s="21"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="B40" s="34" t="s">
-        <v>506</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>288</v>
+        <v>389</v>
+      </c>
+      <c r="B40" s="38" t="s">
+        <v>515</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>390</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E40" s="21"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="33" t="s">
-        <v>406</v>
-      </c>
-      <c r="B41" s="34" t="s">
-        <v>413</v>
+    <row r="41" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" s="38" t="s">
+        <v>394</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="D41" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="E41" s="21"/>
-    </row>
-    <row r="42" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="B42" s="34" t="s">
-        <v>411</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="D42" s="29" t="s">
-        <v>403</v>
-      </c>
-      <c r="E42" s="18"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="33" t="s">
+        <v>387</v>
+      </c>
+      <c r="D41" s="29" t="s">
+        <v>386</v>
+      </c>
+      <c r="E41" s="18"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="34" t="s">
-        <v>466</v>
-      </c>
-      <c r="C43" s="3" t="s">
+      <c r="B42" s="38" t="s">
+        <v>445</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D42" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="D43" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="E43" s="21"/>
-    </row>
-    <row r="44" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="34" t="s">
+      <c r="E42" s="21"/>
+    </row>
+    <row r="43" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="B44" s="34" t="s">
-        <v>484</v>
-      </c>
-      <c r="C44" s="4" t="s">
+      <c r="B43" s="38" t="s">
+        <v>461</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="E44" s="18"/>
+      <c r="D43" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E43" s="18"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="33" t="s">
+        <v>299</v>
+      </c>
+      <c r="B44" s="38" t="s">
+        <v>477</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="D44" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="E44" s="21"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="33" t="s">
-        <v>308</v>
-      </c>
-      <c r="B45" s="34" t="s">
-        <v>500</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>307</v>
+        <v>328</v>
+      </c>
+      <c r="B45" s="38" t="s">
+        <v>434</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>358</v>
       </c>
       <c r="D45" s="28" t="s">
-        <v>306</v>
+        <v>327</v>
       </c>
       <c r="E45" s="21"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="33" t="s">
-        <v>340</v>
-      </c>
-      <c r="B46" s="34" t="s">
-        <v>454</v>
+        <v>479</v>
+      </c>
+      <c r="B46" s="38" t="s">
+        <v>473</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>373</v>
+        <v>487</v>
       </c>
       <c r="D46" s="28" t="s">
-        <v>339</v>
+        <v>480</v>
       </c>
       <c r="E46" s="21"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="33" t="s">
-        <v>504</v>
-      </c>
-      <c r="B47" s="34" t="s">
-        <v>496</v>
+    <row r="47" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="38" t="s">
+        <v>465</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>516</v>
-      </c>
-      <c r="D47" s="28" t="s">
-        <v>505</v>
-      </c>
-      <c r="E47" s="21"/>
-    </row>
-    <row r="48" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="B48" s="34" t="s">
-        <v>488</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="D48" s="29" t="s">
-        <v>342</v>
-      </c>
-      <c r="E48" s="18"/>
-    </row>
-    <row r="49" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="35" t="s">
-        <v>154</v>
-      </c>
-      <c r="B49" s="35"/>
-      <c r="C49" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D49" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="E49" s="19"/>
-    </row>
-    <row r="50" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="36" t="s">
-        <v>319</v>
-      </c>
-      <c r="B50" s="36" t="s">
-        <v>473</v>
-      </c>
-      <c r="C50" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="D50" s="31" t="s">
-        <v>320</v>
-      </c>
-      <c r="E50" s="20"/>
+        <v>330</v>
+      </c>
+      <c r="D47" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="E47" s="18"/>
+    </row>
+    <row r="48" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="B48" s="42"/>
+      <c r="C48" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="E48" s="19"/>
+    </row>
+    <row r="49" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="36" t="s">
+        <v>307</v>
+      </c>
+      <c r="B49" s="43" t="s">
+        <v>451</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="D49" s="31" t="s">
+        <v>308</v>
+      </c>
+      <c r="E49" s="20"/>
+    </row>
+    <row r="50" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B50" s="38" t="s">
+        <v>510</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D50" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="E50" s="18"/>
     </row>
     <row r="51" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="B51" s="34" t="s">
-        <v>350</v>
+        <v>261</v>
+      </c>
+      <c r="B51" s="38" t="s">
+        <v>274</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D51" s="29" t="s">
-        <v>102</v>
+        <v>262</v>
+      </c>
+      <c r="D51" s="28" t="s">
+        <v>263</v>
       </c>
       <c r="E51" s="18"/>
     </row>
     <row r="52" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="34" t="s">
-        <v>270</v>
-      </c>
-      <c r="B52" s="34" t="s">
-        <v>283</v>
+        <v>403</v>
+      </c>
+      <c r="B52" s="38" t="s">
+        <v>406</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>271</v>
+        <v>405</v>
       </c>
       <c r="D52" s="28" t="s">
-        <v>272</v>
+        <v>404</v>
       </c>
       <c r="E52" s="18"/>
     </row>
-    <row r="53" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="34" t="s">
-        <v>422</v>
-      </c>
-      <c r="B53" s="34" t="s">
-        <v>425</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>424</v>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="33" t="s">
+        <v>243</v>
+      </c>
+      <c r="B53" s="38" t="s">
+        <v>249</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>423</v>
-      </c>
-      <c r="E53" s="18"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B54" s="34" t="s">
-        <v>231</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D54" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="E54" s="21"/>
+        <v>244</v>
+      </c>
+      <c r="E53" s="21"/>
+    </row>
+    <row r="54" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="35" t="s">
+        <v>171</v>
+      </c>
+      <c r="B54" s="42"/>
+      <c r="C54" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E54" s="19"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="33" t="s">
-        <v>252</v>
-      </c>
-      <c r="B55" s="34" t="s">
-        <v>258</v>
+        <v>162</v>
+      </c>
+      <c r="B55" s="38" t="s">
+        <v>223</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>106</v>
+        <v>166</v>
       </c>
       <c r="D55" s="28" t="s">
-        <v>253</v>
+        <v>165</v>
       </c>
       <c r="E55" s="21"/>
     </row>
-    <row r="56" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="35" t="s">
-        <v>174</v>
-      </c>
-      <c r="B56" s="35"/>
-      <c r="C56" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="D56" s="30" t="s">
-        <v>175</v>
-      </c>
-      <c r="E56" s="19"/>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="33" t="s">
+        <v>337</v>
+      </c>
+      <c r="B56" s="38" t="s">
+        <v>454</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="D56" s="28" t="s">
+        <v>338</v>
+      </c>
+      <c r="E56" s="21"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="33" t="s">
-        <v>165</v>
-      </c>
-      <c r="B57" s="34" t="s">
-        <v>232</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>169</v>
+        <v>319</v>
+      </c>
+      <c r="B57" s="38" t="s">
+        <v>320</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>322</v>
       </c>
       <c r="D57" s="28" t="s">
-        <v>168</v>
+        <v>321</v>
       </c>
       <c r="E57" s="21"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="33" t="s">
-        <v>351</v>
-      </c>
-      <c r="B58" s="34" t="s">
-        <v>477</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>353</v>
+        <v>163</v>
+      </c>
+      <c r="B58" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>352</v>
+        <v>164</v>
       </c>
       <c r="E58" s="21"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="33" t="s">
-        <v>331</v>
-      </c>
-      <c r="B59" s="34" t="s">
-        <v>332</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>334</v>
+        <v>31</v>
+      </c>
+      <c r="B59" s="38" t="s">
+        <v>323</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="D59" s="28" t="s">
-        <v>333</v>
+        <v>76</v>
       </c>
       <c r="E59" s="21"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="33" t="s">
-        <v>166</v>
-      </c>
-      <c r="B60" s="34" t="s">
-        <v>260</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>117</v>
+        <v>353</v>
+      </c>
+      <c r="B60" s="38" t="s">
+        <v>420</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>355</v>
       </c>
       <c r="D60" s="28" t="s">
-        <v>167</v>
+        <v>354</v>
       </c>
       <c r="E60" s="21"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="B61" s="34" t="s">
-        <v>335</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D61" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="E61" s="21"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="33" t="s">
-        <v>368</v>
-      </c>
-      <c r="B62" s="34" t="s">
-        <v>440</v>
+    <row r="61" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="B61" s="38" t="s">
+        <v>458</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D61" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="E61" s="18"/>
+    </row>
+    <row r="62" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="34" t="s">
+        <v>310</v>
+      </c>
+      <c r="B62" s="38" t="s">
+        <v>449</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="D62" s="28" t="s">
-        <v>369</v>
-      </c>
-      <c r="E62" s="21"/>
-    </row>
-    <row r="63" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="34" t="s">
-        <v>152</v>
-      </c>
-      <c r="B63" s="34" t="s">
-        <v>481</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D63" s="29" t="s">
-        <v>238</v>
-      </c>
-      <c r="E63" s="18"/>
+        <v>311</v>
+      </c>
+      <c r="D62" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="E62" s="18"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="33" t="s">
+        <v>210</v>
+      </c>
+      <c r="B63" s="38" t="s">
+        <v>257</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D63" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="E63" s="22"/>
     </row>
     <row r="64" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="34" t="s">
-        <v>322</v>
-      </c>
-      <c r="B64" s="34" t="s">
-        <v>470</v>
+        <v>191</v>
+      </c>
+      <c r="B64" s="38" t="s">
+        <v>245</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>323</v>
+        <v>199</v>
       </c>
       <c r="D64" s="29" t="s">
-        <v>324</v>
+        <v>198</v>
       </c>
       <c r="E64" s="18"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="33" t="s">
-        <v>218</v>
-      </c>
-      <c r="B65" s="34" t="s">
-        <v>266</v>
+        <v>32</v>
+      </c>
+      <c r="B65" s="38" t="s">
+        <v>252</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>219</v>
+        <v>103</v>
       </c>
       <c r="D65" s="28" t="s">
-        <v>220</v>
-      </c>
-      <c r="E65" s="22"/>
-    </row>
-    <row r="66" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="34" t="s">
-        <v>195</v>
-      </c>
-      <c r="B66" s="34" t="s">
-        <v>254</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="D66" s="29" t="s">
-        <v>204</v>
-      </c>
-      <c r="E66" s="18"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="E65" s="21"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="B66" s="38" t="s">
+        <v>450</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D66" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="E66" s="21"/>
+    </row>
+    <row r="67" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B67" s="34" t="s">
-        <v>261</v>
-      </c>
-      <c r="C67" s="3" t="s">
+      <c r="B67" s="38" t="s">
+        <v>275</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D67" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="E67" s="18"/>
+    </row>
+    <row r="68" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="34" t="s">
+        <v>356</v>
+      </c>
+      <c r="B68" s="38" t="s">
+        <v>357</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="D68" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="E68" s="18"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="B69" s="38" t="s">
+        <v>511</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D69" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="E69" s="21"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B70" s="38" t="s">
+        <v>446</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D70" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="D67" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="E67" s="21"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="33" t="s">
-        <v>280</v>
-      </c>
-      <c r="B68" s="34" t="s">
-        <v>472</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="D68" s="28" t="s">
-        <v>290</v>
-      </c>
-      <c r="E68" s="21"/>
-    </row>
-    <row r="69" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="B69" s="34" t="s">
-        <v>284</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D69" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="E69" s="18"/>
-    </row>
-    <row r="70" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="34" t="s">
-        <v>371</v>
-      </c>
-      <c r="B70" s="34" t="s">
-        <v>372</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>375</v>
-      </c>
-      <c r="D70" s="29" t="s">
-        <v>374</v>
-      </c>
-      <c r="E70" s="18"/>
+      <c r="E70" s="21"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="B71" s="34" t="s">
-        <v>402</v>
+        <v>488</v>
+      </c>
+      <c r="B71" s="38" t="s">
+        <v>489</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>173</v>
+        <v>103</v>
       </c>
       <c r="D71" s="28" t="s">
-        <v>164</v>
+        <v>490</v>
       </c>
       <c r="E71" s="21"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="33" t="s">
+    <row r="72" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="B72" s="38" t="s">
+        <v>396</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D72" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E72" s="18"/>
+    </row>
+    <row r="73" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="B72" s="34" t="s">
-        <v>467</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D72" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="E72" s="21"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="33" t="s">
-        <v>519</v>
-      </c>
-      <c r="B73" s="34" t="s">
-        <v>520</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D73" s="28" t="s">
-        <v>521</v>
-      </c>
-      <c r="E73" s="21"/>
+      <c r="B73" s="38" t="s">
+        <v>396</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D73" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E73" s="18"/>
     </row>
     <row r="74" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="34" t="s">
-        <v>234</v>
-      </c>
-      <c r="B74" s="34" t="s">
-        <v>415</v>
+        <v>508</v>
+      </c>
+      <c r="B74" s="38" t="s">
+        <v>518</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>84</v>
+        <v>412</v>
       </c>
       <c r="D74" s="29" t="s">
-        <v>85</v>
+        <v>509</v>
       </c>
       <c r="E74" s="18"/>
     </row>
     <row r="75" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="B75" s="34" t="s">
-        <v>415</v>
+        <v>239</v>
+      </c>
+      <c r="B75" s="38" t="s">
+        <v>240</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>84</v>
+        <v>241</v>
       </c>
       <c r="D75" s="29" t="s">
-        <v>85</v>
+        <v>242</v>
       </c>
       <c r="E75" s="18"/>
     </row>
-    <row r="76" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="34" t="s">
-        <v>248</v>
-      </c>
-      <c r="B76" s="34" t="s">
-        <v>249</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="D76" s="29" t="s">
-        <v>251</v>
-      </c>
-      <c r="E76" s="18"/>
-    </row>
-    <row r="77" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="B77" s="35"/>
-      <c r="C77" s="7" t="s">
+    <row r="76" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B76" s="42"/>
+      <c r="C76" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D77" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="E77" s="19"/>
+      <c r="D76" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="E76" s="19"/>
+    </row>
+    <row r="77" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="B77" s="38" t="s">
+        <v>397</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D77" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="E77" s="18"/>
     </row>
     <row r="78" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="34" t="s">
-        <v>212</v>
-      </c>
-      <c r="B78" s="34" t="s">
-        <v>416</v>
+        <v>130</v>
+      </c>
+      <c r="B78" s="38" t="s">
+        <v>287</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>125</v>
+        <v>9</v>
       </c>
       <c r="D78" s="29" t="s">
-        <v>213</v>
+        <v>131</v>
       </c>
       <c r="E78" s="18"/>
     </row>
     <row r="79" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="B79" s="34" t="s">
-        <v>296</v>
+        <v>132</v>
+      </c>
+      <c r="B79" s="38" t="s">
+        <v>235</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D79" s="29" t="s">
-        <v>134</v>
-      </c>
-      <c r="E79" s="18"/>
+        <v>133</v>
+      </c>
+      <c r="E79" s="23"/>
     </row>
     <row r="80" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="34" t="s">
-        <v>135</v>
-      </c>
-      <c r="B80" s="34" t="s">
-        <v>244</v>
+        <v>483</v>
+      </c>
+      <c r="B80" s="38" t="s">
+        <v>486</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>9</v>
+        <v>484</v>
       </c>
       <c r="D80" s="29" t="s">
-        <v>136</v>
+        <v>485</v>
       </c>
       <c r="E80" s="23"/>
     </row>
-    <row r="81" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="34" t="s">
-        <v>512</v>
-      </c>
-      <c r="B81" s="34" t="s">
-        <v>515</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>513</v>
+    <row r="81" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="36" t="s">
+        <v>185</v>
+      </c>
+      <c r="B81" s="43" t="s">
+        <v>375</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>285</v>
       </c>
       <c r="D81" s="29" t="s">
-        <v>514</v>
-      </c>
-      <c r="E81" s="23"/>
-    </row>
-    <row r="82" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="36" t="s">
-        <v>189</v>
-      </c>
-      <c r="B82" s="36" t="s">
-        <v>391</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="D82" s="29" t="s">
-        <v>293</v>
-      </c>
-      <c r="E82" s="20"/>
-    </row>
-    <row r="83" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="35" t="s">
-        <v>145</v>
-      </c>
-      <c r="B83" s="35"/>
-      <c r="C83" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="E81" s="20"/>
+    </row>
+    <row r="82" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="B82" s="42"/>
+      <c r="C82" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D83" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="E83" s="24"/>
-    </row>
-    <row r="84" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="34" t="s">
-        <v>392</v>
-      </c>
-      <c r="B84" s="34" t="s">
-        <v>393</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="D84" s="29" t="s">
-        <v>395</v>
-      </c>
-      <c r="E84" s="20"/>
+      <c r="D82" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="E82" s="24"/>
+    </row>
+    <row r="83" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="34" t="s">
+        <v>376</v>
+      </c>
+      <c r="B83" s="38" t="s">
+        <v>377</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="D83" s="29" t="s">
+        <v>379</v>
+      </c>
+      <c r="E83" s="20"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B84" s="38" t="s">
+        <v>231</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D84" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="E84" s="21"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B85" s="34" t="s">
-        <v>240</v>
+        <v>109</v>
+      </c>
+      <c r="B85" s="38" t="s">
+        <v>256</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>110</v>
       </c>
       <c r="D85" s="28" t="s">
-        <v>239</v>
+        <v>108</v>
       </c>
       <c r="E85" s="21"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="B86" s="34" t="s">
-        <v>265</v>
+        <v>276</v>
+      </c>
+      <c r="B86" s="38" t="s">
+        <v>513</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>113</v>
+        <v>278</v>
       </c>
       <c r="D86" s="28" t="s">
-        <v>111</v>
+        <v>277</v>
       </c>
       <c r="E86" s="21"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="33" t="s">
-        <v>285</v>
-      </c>
-      <c r="B87" s="34" t="s">
-        <v>316</v>
+        <v>37</v>
+      </c>
+      <c r="B87" s="38" t="s">
+        <v>478</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>287</v>
+        <v>38</v>
       </c>
       <c r="D87" s="28" t="s">
-        <v>286</v>
+        <v>232</v>
       </c>
       <c r="E87" s="21"/>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B88" s="34" t="s">
-        <v>501</v>
-      </c>
-      <c r="C88" s="3" t="s">
+    <row r="88" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="B88" s="42"/>
+      <c r="C88" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D88" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="E88" s="19"/>
+    </row>
+    <row r="89" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D88" s="28" t="s">
-        <v>241</v>
-      </c>
-      <c r="E88" s="21"/>
-    </row>
-    <row r="89" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="35" t="s">
-        <v>170</v>
-      </c>
-      <c r="B89" s="35"/>
-      <c r="C89" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="D89" s="30" t="s">
-        <v>171</v>
-      </c>
-      <c r="E89" s="19"/>
+      <c r="B89" s="38" t="s">
+        <v>512</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D89" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="E89" s="18"/>
     </row>
     <row r="90" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="B90" s="34" t="s">
-        <v>439</v>
+        <v>208</v>
+      </c>
+      <c r="B90" s="38" t="s">
+        <v>252</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>114</v>
+        <v>206</v>
       </c>
       <c r="D90" s="29" t="s">
-        <v>115</v>
+        <v>207</v>
       </c>
       <c r="E90" s="18"/>
     </row>
     <row r="91" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="B91" s="34" t="s">
-        <v>261</v>
+        <v>417</v>
+      </c>
+      <c r="B91" s="38" t="s">
+        <v>249</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>214</v>
+        <v>415</v>
       </c>
       <c r="D91" s="29" t="s">
-        <v>215</v>
+        <v>414</v>
       </c>
       <c r="E91" s="18"/>
     </row>
     <row r="92" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="34" t="s">
-        <v>436</v>
-      </c>
-      <c r="B92" s="34" t="s">
-        <v>258</v>
+        <v>40</v>
+      </c>
+      <c r="B92" s="38" t="s">
+        <v>248</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>434</v>
+        <v>247</v>
       </c>
       <c r="D92" s="29" t="s">
-        <v>433</v>
+        <v>246</v>
       </c>
       <c r="E92" s="18"/>
     </row>
@@ -3503,44 +3495,44 @@
       <c r="A93" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="B93" s="34" t="s">
-        <v>257</v>
+      <c r="B93" s="38" t="s">
+        <v>428</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>256</v>
+        <v>114</v>
       </c>
       <c r="D93" s="29" t="s">
-        <v>255</v>
+        <v>113</v>
       </c>
       <c r="E93" s="18"/>
     </row>
-    <row r="94" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="34" t="s">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="B94" s="34" t="s">
-        <v>448</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D94" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="E94" s="18"/>
+      <c r="B94" s="38" t="s">
+        <v>507</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D94" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E94" s="21"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B95" s="38" t="s">
+        <v>507</v>
+      </c>
+      <c r="C95" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B95" s="34" t="s">
-        <v>386</v>
-      </c>
-      <c r="C95" s="3" t="s">
+      <c r="D95" s="28" t="s">
         <v>44</v>
-      </c>
-      <c r="D95" s="28" t="s">
-        <v>45</v>
       </c>
       <c r="E95" s="21"/>
     </row>
@@ -3548,400 +3540,400 @@
       <c r="A96" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="B96" s="34" t="s">
-        <v>386</v>
+      <c r="B96" s="38" t="s">
+        <v>507</v>
       </c>
       <c r="C96" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D96" s="28" t="s">
         <v>44</v>
-      </c>
-      <c r="D96" s="28" t="s">
-        <v>45</v>
       </c>
       <c r="E96" s="21"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B97" s="34" t="s">
-        <v>386</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>44</v>
+        <v>391</v>
+      </c>
+      <c r="B97" s="38" t="s">
+        <v>392</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>393</v>
       </c>
       <c r="D97" s="28" t="s">
-        <v>45</v>
+        <v>418</v>
       </c>
       <c r="E97" s="21"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="33" t="s">
-        <v>408</v>
-      </c>
-      <c r="B98" s="34" t="s">
-        <v>409</v>
-      </c>
-      <c r="C98" s="4" t="s">
-        <v>410</v>
+        <v>141</v>
+      </c>
+      <c r="B98" s="38" t="s">
+        <v>340</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="D98" s="28" t="s">
-        <v>437</v>
-      </c>
-      <c r="E98" s="21"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="B99" s="34" t="s">
-        <v>354</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D99" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="E99" s="22"/>
+        <v>89</v>
+      </c>
+      <c r="E98" s="22"/>
+    </row>
+    <row r="99" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="34" t="s">
+        <v>184</v>
+      </c>
+      <c r="B99" s="38" t="s">
+        <v>398</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D99" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="E99" s="18"/>
     </row>
     <row r="100" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="34" t="s">
-        <v>188</v>
-      </c>
-      <c r="B100" s="34" t="s">
-        <v>417</v>
+        <v>47</v>
+      </c>
+      <c r="B100" s="38" t="s">
+        <v>385</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>187</v>
+        <v>301</v>
       </c>
       <c r="D100" s="29" t="s">
-        <v>186</v>
+        <v>300</v>
       </c>
       <c r="E100" s="18"/>
     </row>
-    <row r="101" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="34" t="s">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="B101" s="38" t="s">
+        <v>336</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D101" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="E101" s="21"/>
+    </row>
+    <row r="102" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="B102" s="38" t="s">
+        <v>250</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D102" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="E102" s="18"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="B103" s="38" t="s">
+        <v>495</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="D103" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="E103" s="22"/>
+    </row>
+    <row r="104" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="B101" s="34" t="s">
-        <v>401</v>
-      </c>
-      <c r="C101" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="D101" s="29" t="s">
-        <v>311</v>
-      </c>
-      <c r="E101" s="18"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="33" t="s">
-        <v>198</v>
-      </c>
-      <c r="B102" s="34" t="s">
-        <v>349</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D102" s="28" t="s">
-        <v>200</v>
-      </c>
-      <c r="E102" s="21"/>
-    </row>
-    <row r="103" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="34" t="s">
-        <v>217</v>
-      </c>
-      <c r="B103" s="34" t="s">
-        <v>259</v>
-      </c>
-      <c r="C103" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="D103" s="29" t="s">
-        <v>215</v>
-      </c>
-      <c r="E103" s="18"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="33" t="s">
-        <v>196</v>
-      </c>
-      <c r="B104" s="34" t="s">
-        <v>522</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>523</v>
-      </c>
-      <c r="D104" s="28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E104" s="22"/>
+      <c r="B104" s="38" t="s">
+        <v>466</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D104" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E104" s="18"/>
     </row>
     <row r="105" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="B105" s="34" t="s">
-        <v>489</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>50</v>
+        <v>295</v>
+      </c>
+      <c r="B105" s="38" t="s">
+        <v>457</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>370</v>
       </c>
       <c r="D105" s="29" t="s">
-        <v>86</v>
+        <v>476</v>
       </c>
       <c r="E105" s="18"/>
     </row>
     <row r="106" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="34" t="s">
-        <v>304</v>
-      </c>
-      <c r="B106" s="34" t="s">
-        <v>480</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>385</v>
+        <v>134</v>
+      </c>
+      <c r="B106" s="38" t="s">
+        <v>294</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="D106" s="29" t="s">
-        <v>499</v>
+        <v>135</v>
       </c>
       <c r="E106" s="18"/>
     </row>
     <row r="107" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="B107" s="34" t="s">
-        <v>303</v>
+        <v>332</v>
+      </c>
+      <c r="B107" s="38" t="s">
+        <v>333</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>9</v>
+        <v>334</v>
       </c>
       <c r="D107" s="29" t="s">
-        <v>138</v>
+        <v>335</v>
       </c>
       <c r="E107" s="18"/>
     </row>
     <row r="108" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="34" t="s">
-        <v>345</v>
-      </c>
-      <c r="B108" s="34" t="s">
-        <v>346</v>
+        <v>219</v>
+      </c>
+      <c r="B108" s="38" t="s">
+        <v>384</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>347</v>
+        <v>220</v>
       </c>
       <c r="D108" s="29" t="s">
-        <v>348</v>
+        <v>221</v>
       </c>
       <c r="E108" s="18"/>
     </row>
-    <row r="109" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="34" t="s">
-        <v>227</v>
-      </c>
-      <c r="B109" s="34" t="s">
-        <v>400</v>
-      </c>
-      <c r="C109" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="D109" s="29" t="s">
-        <v>229</v>
-      </c>
-      <c r="E109" s="18"/>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B109" s="38" t="s">
+        <v>293</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D109" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="E109" s="22"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="33" t="s">
+      <c r="A110" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="B110" s="34" t="s">
-        <v>302</v>
+      <c r="B110" s="38" t="s">
+        <v>325</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>118</v>
+        <v>259</v>
       </c>
       <c r="D110" s="28" t="s">
-        <v>242</v>
-      </c>
-      <c r="E110" s="22"/>
+        <v>258</v>
+      </c>
+      <c r="E110" s="21"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="B111" s="34" t="s">
-        <v>337</v>
+      <c r="A111" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="B111" s="38" t="s">
+        <v>226</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>268</v>
+        <v>217</v>
       </c>
       <c r="D111" s="28" t="s">
-        <v>267</v>
+        <v>218</v>
       </c>
       <c r="E111" s="21"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="33" t="s">
-        <v>224</v>
-      </c>
-      <c r="B112" s="34" t="s">
-        <v>235</v>
-      </c>
-      <c r="C112" s="3" t="s">
-        <v>225</v>
+        <v>350</v>
+      </c>
+      <c r="B112" s="38" t="s">
+        <v>453</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>352</v>
       </c>
       <c r="D112" s="28" t="s">
-        <v>226</v>
+        <v>351</v>
       </c>
       <c r="E112" s="21"/>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="33" t="s">
-        <v>365</v>
-      </c>
-      <c r="B113" s="34" t="s">
-        <v>476</v>
-      </c>
-      <c r="C113" s="4" t="s">
-        <v>367</v>
-      </c>
-      <c r="D113" s="28" t="s">
-        <v>366</v>
-      </c>
-      <c r="E113" s="21"/>
-    </row>
-    <row r="114" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="35" t="s">
-        <v>177</v>
-      </c>
-      <c r="B114" s="35"/>
-      <c r="C114" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="D114" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="E114" s="19"/>
+    <row r="113" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="B113" s="42"/>
+      <c r="C113" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D113" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="E113" s="19"/>
+    </row>
+    <row r="114" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B114" s="38" t="s">
+        <v>380</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D114" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="E114" s="18"/>
     </row>
     <row r="115" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="B115" s="34" t="s">
-        <v>396</v>
+        <v>264</v>
+      </c>
+      <c r="B115" s="38" t="s">
+        <v>265</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D115" s="29" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E115" s="18"/>
     </row>
     <row r="116" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="34" t="s">
-        <v>273</v>
-      </c>
-      <c r="B116" s="34" t="s">
-        <v>274</v>
+        <v>421</v>
+      </c>
+      <c r="B116" s="38" t="s">
+        <v>447</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>119</v>
+        <v>427</v>
       </c>
       <c r="D116" s="29" t="s">
-        <v>143</v>
+        <v>426</v>
       </c>
       <c r="E116" s="18"/>
     </row>
     <row r="117" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="34" t="s">
-        <v>441</v>
-      </c>
-      <c r="B117" s="34" t="s">
-        <v>468</v>
+        <v>381</v>
+      </c>
+      <c r="B117" s="38" t="s">
+        <v>382</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>447</v>
+        <v>116</v>
       </c>
       <c r="D117" s="29" t="s">
-        <v>446</v>
+        <v>140</v>
       </c>
       <c r="E117" s="18"/>
     </row>
-    <row r="118" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="34" t="s">
-        <v>397</v>
-      </c>
-      <c r="B118" s="34" t="s">
-        <v>398</v>
-      </c>
-      <c r="C118" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D118" s="29" t="s">
+    <row r="118" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="E118" s="18"/>
-    </row>
-    <row r="119" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="37" t="s">
+      <c r="B118" s="43" t="s">
+        <v>388</v>
+      </c>
+      <c r="C118" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D118" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="B119" s="36" t="s">
-        <v>405</v>
-      </c>
-      <c r="C119" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="D119" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="E119" s="25"/>
-    </row>
-    <row r="120" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="35" t="s">
+      <c r="E118" s="25"/>
+    </row>
+    <row r="119" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B119" s="42"/>
+      <c r="C119" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D119" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="E119" s="24"/>
+    </row>
+    <row r="120" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="34" t="s">
+        <v>342</v>
+      </c>
+      <c r="B120" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="C120" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D120" s="29" t="s">
+        <v>343</v>
+      </c>
+      <c r="E120" s="20"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="B120" s="35"/>
-      <c r="C120" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D120" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="E120" s="24"/>
-    </row>
-    <row r="121" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="34" t="s">
-        <v>357</v>
-      </c>
-      <c r="B121" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="C121" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="D121" s="29" t="s">
-        <v>358</v>
-      </c>
-      <c r="E121" s="20"/>
+      <c r="B121" s="38" t="s">
+        <v>517</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D121" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="E121" s="21"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="B122" s="34" t="s">
-        <v>518</v>
+      <c r="B122" s="38" t="s">
+        <v>517</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D122" s="28" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E122" s="21"/>
     </row>
@@ -3949,14 +3941,14 @@
       <c r="A123" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="B123" s="34" t="s">
-        <v>518</v>
+      <c r="B123" s="38" t="s">
+        <v>517</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D123" s="28" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E123" s="21"/>
     </row>
@@ -3964,14 +3956,14 @@
       <c r="A124" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="B124" s="34" t="s">
-        <v>518</v>
+      <c r="B124" s="38" t="s">
+        <v>517</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D124" s="28" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E124" s="21"/>
     </row>
@@ -3979,59 +3971,59 @@
       <c r="A125" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="B125" s="34" t="s">
-        <v>518</v>
+      <c r="B125" s="38" t="s">
+        <v>517</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D125" s="28" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E125" s="21"/>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="B126" s="34" t="s">
-        <v>518</v>
+        <v>269</v>
+      </c>
+      <c r="B126" s="38" t="s">
+        <v>519</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>120</v>
+        <v>268</v>
       </c>
       <c r="D126" s="28" t="s">
-        <v>121</v>
+        <v>267</v>
       </c>
       <c r="E126" s="21"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="33" t="s">
-        <v>278</v>
-      </c>
-      <c r="B127" s="34" t="s">
-        <v>474</v>
+        <v>313</v>
+      </c>
+      <c r="B127" s="38" t="s">
+        <v>304</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>277</v>
+        <v>315</v>
       </c>
       <c r="D127" s="28" t="s">
-        <v>276</v>
+        <v>314</v>
       </c>
       <c r="E127" s="21"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="33" t="s">
-        <v>325</v>
-      </c>
-      <c r="B128" s="34" t="s">
-        <v>315</v>
+        <v>60</v>
+      </c>
+      <c r="B128" s="38" t="s">
+        <v>224</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>327</v>
+        <v>29</v>
       </c>
       <c r="D128" s="28" t="s">
-        <v>326</v>
+        <v>119</v>
       </c>
       <c r="E128" s="21"/>
     </row>
@@ -4039,601 +4031,587 @@
       <c r="A129" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="B129" s="34" t="s">
-        <v>233</v>
+      <c r="B129" s="38" t="s">
+        <v>456</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>29</v>
+        <v>120</v>
       </c>
       <c r="D129" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="E129" s="21"/>
+        <v>234</v>
+      </c>
+      <c r="E129" s="22"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="33" t="s">
+        <v>288</v>
+      </c>
+      <c r="B130" s="38" t="s">
+        <v>419</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D130" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="E130" s="22"/>
+    </row>
+    <row r="131" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="B130" s="34" t="s">
-        <v>479</v>
-      </c>
-      <c r="C130" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D130" s="28" t="s">
-        <v>243</v>
-      </c>
-      <c r="E130" s="22"/>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A131" s="33" t="s">
-        <v>297</v>
-      </c>
-      <c r="B131" s="34" t="s">
-        <v>438</v>
-      </c>
-      <c r="C131" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="D131" s="28" t="s">
-        <v>300</v>
-      </c>
-      <c r="E131" s="22"/>
+      <c r="B131" s="38" t="s">
+        <v>482</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D131" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E131" s="18"/>
     </row>
     <row r="132" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="B132" s="34" t="s">
-        <v>511</v>
+        <v>253</v>
+      </c>
+      <c r="B132" s="38" t="s">
+        <v>254</v>
       </c>
       <c r="C132" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D132" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="E132" s="18"/>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="B133" s="38" t="s">
+        <v>260</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D133" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="E133" s="21"/>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" s="33" t="s">
+        <v>438</v>
+      </c>
+      <c r="B134" s="38" t="s">
+        <v>440</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="D134" s="28" t="s">
+        <v>439</v>
+      </c>
+      <c r="E134" s="21"/>
+    </row>
+    <row r="135" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="34" t="s">
+        <v>407</v>
+      </c>
+      <c r="B135" s="38" t="s">
+        <v>448</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="D135" s="29" t="s">
+        <v>408</v>
+      </c>
+      <c r="E135" s="18"/>
+    </row>
+    <row r="136" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="B136" s="38" t="s">
+        <v>383</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D136" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="E136" s="18"/>
+    </row>
+    <row r="137" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="B137" s="43" t="s">
+        <v>452</v>
+      </c>
+      <c r="C137" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D137" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="E137" s="20"/>
+      <c r="F137" s="16"/>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="D132" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="E132" s="18"/>
-    </row>
-    <row r="133" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="34" t="s">
-        <v>203</v>
-      </c>
-      <c r="B133" s="34" t="s">
-        <v>355</v>
-      </c>
-      <c r="C133" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D133" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="E133" s="18"/>
-    </row>
-    <row r="134" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="34" t="s">
-        <v>262</v>
-      </c>
-      <c r="B134" s="34" t="s">
-        <v>263</v>
-      </c>
-      <c r="C134" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D134" s="29" t="s">
-        <v>264</v>
-      </c>
-      <c r="E134" s="18"/>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="B135" s="34" t="s">
-        <v>269</v>
-      </c>
-      <c r="C135" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D135" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="E135" s="21"/>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" s="33" t="s">
-        <v>458</v>
-      </c>
-      <c r="B136" s="34" t="s">
-        <v>460</v>
-      </c>
-      <c r="C136" s="3" t="s">
-        <v>461</v>
-      </c>
-      <c r="D136" s="28" t="s">
-        <v>459</v>
-      </c>
-      <c r="E136" s="21"/>
-    </row>
-    <row r="137" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="34" t="s">
-        <v>426</v>
-      </c>
-      <c r="B137" s="34" t="s">
-        <v>469</v>
-      </c>
-      <c r="C137" s="4" t="s">
-        <v>428</v>
-      </c>
-      <c r="D137" s="29" t="s">
-        <v>427</v>
-      </c>
-      <c r="E137" s="18"/>
-    </row>
-    <row r="138" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="34" t="s">
-        <v>191</v>
-      </c>
-      <c r="B138" s="34" t="s">
-        <v>399</v>
-      </c>
-      <c r="C138" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="D138" s="29" t="s">
-        <v>190</v>
-      </c>
-      <c r="E138" s="18"/>
-    </row>
-    <row r="139" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="36" t="s">
-        <v>150</v>
-      </c>
-      <c r="B139" s="36" t="s">
-        <v>475</v>
-      </c>
-      <c r="C139" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="D139" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="E139" s="20"/>
-      <c r="F139" s="16"/>
+      <c r="B138" s="38" t="s">
+        <v>273</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D138" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="E138" s="21"/>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" s="33" t="s">
+        <v>154</v>
+      </c>
+      <c r="B139" s="38" t="s">
+        <v>227</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D139" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="E139" s="21"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="B140" s="34" t="s">
+        <v>237</v>
+      </c>
+      <c r="B140" s="38" t="s">
         <v>282</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D140" s="28" t="s">
-        <v>124</v>
+        <v>238</v>
       </c>
       <c r="E140" s="21"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="33" t="s">
-        <v>157</v>
-      </c>
-      <c r="B141" s="34" t="s">
-        <v>236</v>
+        <v>411</v>
+      </c>
+      <c r="B141" s="38" t="s">
+        <v>436</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>125</v>
+        <v>412</v>
       </c>
       <c r="D141" s="28" t="s">
-        <v>158</v>
+        <v>410</v>
       </c>
       <c r="E141" s="21"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="33" t="s">
-        <v>246</v>
-      </c>
-      <c r="B142" s="34" t="s">
-        <v>291</v>
+        <v>474</v>
+      </c>
+      <c r="B142" s="38" t="s">
+        <v>475</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>125</v>
+        <v>472</v>
       </c>
       <c r="D142" s="28" t="s">
-        <v>247</v>
+        <v>471</v>
       </c>
       <c r="E142" s="21"/>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A143" s="33" t="s">
-        <v>430</v>
-      </c>
-      <c r="B143" s="34" t="s">
-        <v>471</v>
-      </c>
-      <c r="C143" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="D143" s="28" t="s">
-        <v>429</v>
-      </c>
-      <c r="E143" s="21"/>
+    <row r="143" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B143" s="38" t="s">
+        <v>235</v>
+      </c>
+      <c r="C143" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D143" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="E143" s="18"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="33" t="s">
-        <v>497</v>
-      </c>
-      <c r="B144" s="34" t="s">
-        <v>498</v>
+        <v>65</v>
+      </c>
+      <c r="B144" s="38" t="s">
+        <v>395</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>495</v>
+        <v>52</v>
       </c>
       <c r="D144" s="28" t="s">
-        <v>494</v>
+        <v>123</v>
       </c>
       <c r="E144" s="21"/>
     </row>
-    <row r="145" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="34" t="s">
-        <v>139</v>
-      </c>
-      <c r="B145" s="34" t="s">
-        <v>244</v>
-      </c>
-      <c r="C145" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D145" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="E145" s="18"/>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="33" t="s">
+        <v>399</v>
+      </c>
+      <c r="B145" s="38" t="s">
+        <v>402</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D145" s="28" t="s">
+        <v>400</v>
+      </c>
+      <c r="E145" s="21"/>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="B146" s="34" t="s">
-        <v>412</v>
+        <v>70</v>
+      </c>
+      <c r="B146" s="38" t="s">
+        <v>228</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D146" s="28" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E146" s="21"/>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="33" t="s">
-        <v>418</v>
-      </c>
-      <c r="B147" s="34" t="s">
-        <v>421</v>
+        <v>66</v>
+      </c>
+      <c r="B147" s="38" t="s">
+        <v>504</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>420</v>
+        <v>67</v>
       </c>
       <c r="D147" s="28" t="s">
-        <v>419</v>
-      </c>
-      <c r="E147" s="21"/>
+        <v>124</v>
+      </c>
+      <c r="E147" s="22"/>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="B148" s="34" t="s">
-        <v>237</v>
-      </c>
-      <c r="C148" s="3" t="s">
-        <v>53</v>
+        <v>361</v>
+      </c>
+      <c r="B148" s="38" t="s">
+        <v>364</v>
+      </c>
+      <c r="C148" s="4" t="s">
+        <v>363</v>
       </c>
       <c r="D148" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="E148" s="21"/>
+        <v>362</v>
+      </c>
+      <c r="E148" s="22"/>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="B149" s="34" t="s">
-        <v>465</v>
-      </c>
-      <c r="C149" s="3" t="s">
-        <v>68</v>
+        <v>500</v>
+      </c>
+      <c r="B149" s="38" t="s">
+        <v>245</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>502</v>
       </c>
       <c r="D149" s="28" t="s">
-        <v>127</v>
+        <v>501</v>
       </c>
       <c r="E149" s="22"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="33" t="s">
-        <v>376</v>
-      </c>
-      <c r="B150" s="34" t="s">
-        <v>379</v>
+        <v>346</v>
+      </c>
+      <c r="B150" s="38" t="s">
+        <v>499</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>378</v>
+        <v>347</v>
       </c>
       <c r="D150" s="28" t="s">
-        <v>377</v>
+        <v>348</v>
       </c>
       <c r="E150" s="22"/>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A151" s="33" t="s">
-        <v>361</v>
-      </c>
-      <c r="B151" s="39">
-        <v>3966</v>
-      </c>
-      <c r="C151" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="D151" s="28" t="s">
-        <v>363</v>
-      </c>
-      <c r="E151" s="22"/>
-    </row>
-    <row r="152" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="35" t="s">
-        <v>206</v>
-      </c>
-      <c r="B152" s="35"/>
-      <c r="C152" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="D152" s="30" t="s">
-        <v>207</v>
-      </c>
-      <c r="E152" s="19"/>
+    <row r="151" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="35" t="s">
+        <v>200</v>
+      </c>
+      <c r="B151" s="42"/>
+      <c r="C151" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D151" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="E151" s="19"/>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B152" s="38" t="s">
+        <v>345</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D152" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="E152" s="21"/>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="33" t="s">
+        <v>481</v>
+      </c>
+      <c r="B153" s="38" t="s">
+        <v>498</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D153" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E153" s="21"/>
+    </row>
+    <row r="154" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="B153" s="34" t="s">
-        <v>360</v>
-      </c>
-      <c r="C153" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D153" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="E153" s="21"/>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A154" s="33" t="s">
-        <v>509</v>
-      </c>
-      <c r="B154" s="34" t="s">
-        <v>510</v>
-      </c>
-      <c r="C154" s="3" t="s">
+      <c r="B154" s="38" t="s">
+        <v>496</v>
+      </c>
+      <c r="C154" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D154" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="E154" s="21"/>
-    </row>
-    <row r="155" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="B155" s="34" t="s">
-        <v>507</v>
+        <v>82</v>
+      </c>
+      <c r="E154" s="18"/>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="B155" s="40" t="s">
+        <v>497</v>
       </c>
       <c r="C155" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D155" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="E155" s="18"/>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A156" s="33" t="s">
-        <v>223</v>
-      </c>
-      <c r="B156" s="33" t="s">
-        <v>508</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B156" s="38" t="s">
+        <v>324</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="D156" s="29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="E156" s="18"/>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="B157" s="34" t="s">
-        <v>336</v>
-      </c>
-      <c r="C157" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D157" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="E157" s="18"/>
+      <c r="B157" s="38" t="s">
+        <v>305</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D157" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="E157" s="22"/>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="B158" s="34" t="s">
-        <v>317</v>
+      <c r="B158" s="38" t="s">
+        <v>455</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>129</v>
+        <v>38</v>
       </c>
       <c r="D158" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="E158" s="22"/>
+        <v>232</v>
+      </c>
+      <c r="E158" s="21"/>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="B159" s="34" t="s">
-        <v>478</v>
+      <c r="B159" s="38" t="s">
+        <v>349</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>39</v>
+        <v>129</v>
       </c>
       <c r="D159" s="28" t="s">
-        <v>241</v>
-      </c>
-      <c r="E159" s="21"/>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="E159" s="22"/>
+    </row>
+    <row r="160" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="B160" s="34" t="s">
-        <v>364</v>
-      </c>
-      <c r="C160" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D160" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="E160" s="22"/>
+      <c r="B160" s="38" t="s">
+        <v>306</v>
+      </c>
+      <c r="C160" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D160" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E160" s="18"/>
     </row>
     <row r="161" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="B161" s="34" t="s">
-        <v>318</v>
+        <v>203</v>
+      </c>
+      <c r="B161" s="38" t="s">
+        <v>224</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>4</v>
+        <v>506</v>
       </c>
       <c r="D161" s="29" t="s">
-        <v>77</v>
+        <v>505</v>
       </c>
       <c r="E161" s="18"/>
     </row>
-    <row r="162" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="34" t="s">
-        <v>209</v>
-      </c>
-      <c r="B162" s="34" t="s">
-        <v>233</v>
-      </c>
-      <c r="C162" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="D162" s="29" t="s">
-        <v>211</v>
-      </c>
-      <c r="E162" s="18"/>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A163" s="33" t="s">
-        <v>442</v>
-      </c>
-      <c r="B163" s="33" t="s">
-        <v>445</v>
-      </c>
-      <c r="C163" s="3" t="s">
-        <v>444</v>
-      </c>
-      <c r="D163" s="28" t="s">
-        <v>443</v>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="33" t="s">
+        <v>422</v>
+      </c>
+      <c r="B162" s="40" t="s">
+        <v>425</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="D162" s="28" t="s">
+        <v>423</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D94" r:id="rId1"/>
-    <hyperlink ref="D161" r:id="rId2"/>
-    <hyperlink ref="D160" r:id="rId3"/>
-    <hyperlink ref="D158" r:id="rId4"/>
-    <hyperlink ref="D157" r:id="rId5"/>
-    <hyperlink ref="D148" r:id="rId6"/>
-    <hyperlink ref="D155" r:id="rId7"/>
-    <hyperlink ref="D153" r:id="rId8"/>
-    <hyperlink ref="D149" r:id="rId9"/>
-    <hyperlink ref="D146" r:id="rId10"/>
-    <hyperlink ref="D145" r:id="rId11"/>
-    <hyperlink ref="D140" r:id="rId12"/>
-    <hyperlink ref="D86" r:id="rId13"/>
-    <hyperlink ref="D132" r:id="rId14"/>
-    <hyperlink ref="D126" r:id="rId15"/>
-    <hyperlink ref="D83" r:id="rId16"/>
-    <hyperlink ref="D80" r:id="rId17"/>
-    <hyperlink ref="D79" r:id="rId18"/>
-    <hyperlink ref="D77" r:id="rId19"/>
-    <hyperlink ref="D75" r:id="rId20"/>
-    <hyperlink ref="D72" r:id="rId21"/>
-    <hyperlink ref="D74" r:id="rId22"/>
-    <hyperlink ref="D69" r:id="rId23"/>
-    <hyperlink ref="D67" r:id="rId24"/>
-    <hyperlink ref="D61" r:id="rId25"/>
-    <hyperlink ref="D54" r:id="rId26"/>
-    <hyperlink ref="D51" r:id="rId27"/>
-    <hyperlink ref="D49" r:id="rId28"/>
-    <hyperlink ref="D44" r:id="rId29"/>
-    <hyperlink ref="D43" r:id="rId30"/>
-    <hyperlink ref="D40" r:id="rId31"/>
-    <hyperlink ref="D39" r:id="rId32"/>
-    <hyperlink ref="D38" r:id="rId33"/>
-    <hyperlink ref="D36" r:id="rId34"/>
-    <hyperlink ref="D35" r:id="rId35"/>
-    <hyperlink ref="D34" r:id="rId36"/>
-    <hyperlink ref="D33" r:id="rId37"/>
-    <hyperlink ref="D29" r:id="rId38"/>
-    <hyperlink ref="D6" r:id="rId39"/>
-    <hyperlink ref="D15" r:id="rId40"/>
-    <hyperlink ref="D9" r:id="rId41"/>
-    <hyperlink ref="D4" r:id="rId42"/>
-    <hyperlink ref="D3" r:id="rId43"/>
-    <hyperlink ref="D2" r:id="rId44"/>
-    <hyperlink ref="D96" r:id="rId45"/>
-    <hyperlink ref="D125" r:id="rId46"/>
-    <hyperlink ref="D124" r:id="rId47"/>
-    <hyperlink ref="D123" r:id="rId48"/>
-    <hyperlink ref="D122" r:id="rId49"/>
-    <hyperlink ref="D120" r:id="rId50"/>
-    <hyperlink ref="D119" r:id="rId51"/>
-    <hyperlink ref="D107" r:id="rId52"/>
-    <hyperlink ref="D105" r:id="rId53"/>
-    <hyperlink ref="D99" r:id="rId54"/>
-    <hyperlink ref="D97" r:id="rId55"/>
-    <hyperlink ref="D162" r:id="rId56"/>
-    <hyperlink ref="D7" r:id="rId57"/>
-    <hyperlink ref="D5" r:id="rId58"/>
-    <hyperlink ref="D10" r:id="rId59"/>
-    <hyperlink ref="D156" r:id="rId60"/>
-    <hyperlink ref="D85" r:id="rId61"/>
-    <hyperlink ref="D129" r:id="rId62"/>
-    <hyperlink ref="D52" r:id="rId63"/>
-    <hyperlink ref="D87" r:id="rId64"/>
-    <hyperlink ref="D31" r:id="rId65"/>
-    <hyperlink ref="D8" r:id="rId66"/>
-    <hyperlink ref="D95" r:id="rId67"/>
-    <hyperlink ref="D41" r:id="rId68"/>
-    <hyperlink ref="D163" r:id="rId69"/>
-    <hyperlink ref="D27" r:id="rId70"/>
-    <hyperlink ref="D106" r:id="rId71"/>
-    <hyperlink ref="D154" r:id="rId72"/>
+    <hyperlink ref="D93" r:id="rId1"/>
+    <hyperlink ref="D160" r:id="rId2"/>
+    <hyperlink ref="D159" r:id="rId3"/>
+    <hyperlink ref="D157" r:id="rId4"/>
+    <hyperlink ref="D156" r:id="rId5"/>
+    <hyperlink ref="D146" r:id="rId6"/>
+    <hyperlink ref="D154" r:id="rId7"/>
+    <hyperlink ref="D152" r:id="rId8"/>
+    <hyperlink ref="D147" r:id="rId9"/>
+    <hyperlink ref="D144" r:id="rId10"/>
+    <hyperlink ref="D143" r:id="rId11"/>
+    <hyperlink ref="D138" r:id="rId12"/>
+    <hyperlink ref="D85" r:id="rId13"/>
+    <hyperlink ref="D131" r:id="rId14"/>
+    <hyperlink ref="D125" r:id="rId15"/>
+    <hyperlink ref="D82" r:id="rId16"/>
+    <hyperlink ref="D79" r:id="rId17"/>
+    <hyperlink ref="D78" r:id="rId18"/>
+    <hyperlink ref="D76" r:id="rId19"/>
+    <hyperlink ref="D73" r:id="rId20"/>
+    <hyperlink ref="D70" r:id="rId21"/>
+    <hyperlink ref="D72" r:id="rId22"/>
+    <hyperlink ref="D67" r:id="rId23"/>
+    <hyperlink ref="D65" r:id="rId24"/>
+    <hyperlink ref="D59" r:id="rId25"/>
+    <hyperlink ref="D50" r:id="rId26"/>
+    <hyperlink ref="D48" r:id="rId27"/>
+    <hyperlink ref="D43" r:id="rId28"/>
+    <hyperlink ref="D42" r:id="rId29"/>
+    <hyperlink ref="D39" r:id="rId30"/>
+    <hyperlink ref="D38" r:id="rId31"/>
+    <hyperlink ref="D37" r:id="rId32"/>
+    <hyperlink ref="D35" r:id="rId33"/>
+    <hyperlink ref="D34" r:id="rId34"/>
+    <hyperlink ref="D33" r:id="rId35"/>
+    <hyperlink ref="D32" r:id="rId36"/>
+    <hyperlink ref="D28" r:id="rId37"/>
+    <hyperlink ref="D6" r:id="rId38"/>
+    <hyperlink ref="D14" r:id="rId39"/>
+    <hyperlink ref="D9" r:id="rId40"/>
+    <hyperlink ref="D4" r:id="rId41"/>
+    <hyperlink ref="D3" r:id="rId42"/>
+    <hyperlink ref="D2" r:id="rId43"/>
+    <hyperlink ref="D95" r:id="rId44"/>
+    <hyperlink ref="D124" r:id="rId45"/>
+    <hyperlink ref="D123" r:id="rId46"/>
+    <hyperlink ref="D122" r:id="rId47"/>
+    <hyperlink ref="D121" r:id="rId48"/>
+    <hyperlink ref="D119" r:id="rId49"/>
+    <hyperlink ref="D118" r:id="rId50"/>
+    <hyperlink ref="D106" r:id="rId51"/>
+    <hyperlink ref="D104" r:id="rId52"/>
+    <hyperlink ref="D98" r:id="rId53"/>
+    <hyperlink ref="D96" r:id="rId54"/>
+    <hyperlink ref="D7" r:id="rId55"/>
+    <hyperlink ref="D5" r:id="rId56"/>
+    <hyperlink ref="D10" r:id="rId57"/>
+    <hyperlink ref="D155" r:id="rId58"/>
+    <hyperlink ref="D84" r:id="rId59"/>
+    <hyperlink ref="D128" r:id="rId60"/>
+    <hyperlink ref="D51" r:id="rId61"/>
+    <hyperlink ref="D86" r:id="rId62"/>
+    <hyperlink ref="D30" r:id="rId63"/>
+    <hyperlink ref="D8" r:id="rId64"/>
+    <hyperlink ref="D94" r:id="rId65"/>
+    <hyperlink ref="D40" r:id="rId66"/>
+    <hyperlink ref="D162" r:id="rId67"/>
+    <hyperlink ref="D26" r:id="rId68"/>
+    <hyperlink ref="D105" r:id="rId69"/>
+    <hyperlink ref="D153" r:id="rId70"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId73"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId71"/>
+  <ignoredErrors>
+    <ignoredError sqref="B150" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>